<commit_message>
My clustering Algo addedgit add .
</commit_message>
<xml_diff>
--- a/Results-100Nodes.xlsx
+++ b/Results-100Nodes.xlsx
@@ -39,12 +39,6 @@
     <t>Best Sol</t>
   </si>
   <si>
-    <t>AVG KNN Distances</t>
-  </si>
-  <si>
-    <t>AVG KNN CT</t>
-  </si>
-  <si>
     <t>Best KNN Distances</t>
   </si>
   <si>
@@ -232,6 +226,12 @@
   </si>
   <si>
     <t>Total</t>
+  </si>
+  <si>
+    <t>AVG Worse2Worst's Distances</t>
+  </si>
+  <si>
+    <t>AVG Worse2Worst's CT</t>
   </si>
 </sst>
 </file>
@@ -371,9 +371,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -656,8 +654,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AW60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G54" sqref="G54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -686,16 +684,16 @@
       <c r="K1" s="14"/>
       <c r="L1" s="14"/>
       <c r="M1" s="15"/>
-      <c r="N1" s="16" t="s">
-        <v>3</v>
-      </c>
-      <c r="O1" s="16"/>
-      <c r="P1" s="16"/>
-      <c r="Q1" s="16"/>
-      <c r="R1" s="16"/>
-      <c r="S1" s="16"/>
+      <c r="N1" s="13" t="s">
+        <v>69</v>
+      </c>
+      <c r="O1" s="14"/>
+      <c r="P1" s="14"/>
+      <c r="Q1" s="14"/>
+      <c r="R1" s="14"/>
+      <c r="S1" s="14"/>
       <c r="T1" s="13" t="s">
-        <v>4</v>
+        <v>70</v>
       </c>
       <c r="U1" s="14"/>
       <c r="V1" s="14"/>
@@ -703,15 +701,15 @@
       <c r="X1" s="14"/>
       <c r="Y1" s="14"/>
       <c r="Z1" s="13" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="AA1" s="14"/>
       <c r="AB1" s="14"/>
       <c r="AC1" s="14"/>
       <c r="AD1" s="14"/>
-      <c r="AE1" s="14"/>
+      <c r="AE1" s="15"/>
       <c r="AF1" s="13" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="AG1" s="14"/>
       <c r="AH1" s="14"/>
@@ -719,7 +717,7 @@
       <c r="AJ1" s="14"/>
       <c r="AK1" s="14"/>
       <c r="AL1" s="13" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="AM1" s="14"/>
       <c r="AN1" s="14"/>
@@ -727,158 +725,158 @@
       <c r="AP1" s="14"/>
       <c r="AQ1" s="14"/>
       <c r="AR1" s="13" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="AS1" s="14"/>
       <c r="AT1" s="14"/>
       <c r="AU1" s="14"/>
       <c r="AV1" s="14"/>
-      <c r="AW1" s="15"/>
+      <c r="AW1" s="14"/>
     </row>
     <row r="2" spans="1:49" x14ac:dyDescent="0.25">
       <c r="B2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="D2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="E2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="D2" s="3" t="s">
+      <c r="F2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="E2" s="3" t="s">
+      <c r="G2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="F2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="G2" s="4" t="s">
-        <v>70</v>
-      </c>
       <c r="H2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="M2" s="4" t="s">
         <v>68</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="M2" s="4" t="s">
-        <v>70</v>
-      </c>
-      <c r="N2" t="s">
+      <c r="N2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="O2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="P2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="O2" t="s">
+      <c r="Q2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="P2" t="s">
+      <c r="R2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="Q2" t="s">
+      <c r="S2" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="R2" t="s">
-        <v>69</v>
-      </c>
-      <c r="S2" t="s">
-        <v>70</v>
-      </c>
       <c r="T2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="U2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="V2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="U2" s="3" t="s">
+      <c r="W2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="V2" s="3" t="s">
+      <c r="X2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="W2" s="3" t="s">
+      <c r="Y2" s="16" t="s">
         <v>68</v>
       </c>
-      <c r="X2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="Y2" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="Z2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AA2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AB2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AA2" s="3" t="s">
+      <c r="AC2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AB2" s="3" t="s">
+      <c r="AD2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AC2" s="3" t="s">
+      <c r="AE2" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="AD2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AE2" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="AF2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AG2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AH2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AG2" s="3" t="s">
+      <c r="AI2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AH2" s="3" t="s">
+      <c r="AJ2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AI2" s="3" t="s">
+      <c r="AK2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="AJ2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AK2" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="AL2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AM2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AN2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AM2" s="3" t="s">
+      <c r="AO2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AN2" s="3" t="s">
+      <c r="AP2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AO2" s="3" t="s">
+      <c r="AQ2" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="AP2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AQ2" s="3" t="s">
-        <v>70</v>
-      </c>
       <c r="AR2" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="AS2" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="AT2" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="AS2" s="3" t="s">
+      <c r="AU2" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="AT2" s="3" t="s">
+      <c r="AV2" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="AU2" s="3" t="s">
+      <c r="AW2" s="3" t="s">
         <v>68</v>
-      </c>
-      <c r="AV2" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="AW2" s="5" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:49" x14ac:dyDescent="0.25">
@@ -895,7 +893,7 @@
       <c r="K3" s="6"/>
       <c r="L3" s="6"/>
       <c r="M3" s="8"/>
-      <c r="N3" s="6"/>
+      <c r="N3" s="7"/>
       <c r="O3" s="6"/>
       <c r="P3" s="6"/>
       <c r="Q3" s="6"/>
@@ -910,9 +908,9 @@
       <c r="Z3" s="7"/>
       <c r="AA3" s="6"/>
       <c r="AB3" s="6"/>
-      <c r="AC3" s="9"/>
+      <c r="AC3" s="6"/>
       <c r="AD3" s="6"/>
-      <c r="AE3" s="6"/>
+      <c r="AE3" s="8"/>
       <c r="AF3" s="7"/>
       <c r="AG3" s="6"/>
       <c r="AH3" s="6"/>
@@ -922,7 +920,7 @@
       <c r="AL3" s="7"/>
       <c r="AM3" s="6"/>
       <c r="AN3" s="6"/>
-      <c r="AO3" s="6"/>
+      <c r="AO3" s="9"/>
       <c r="AP3" s="6"/>
       <c r="AQ3" s="6"/>
       <c r="AR3" s="7"/>
@@ -930,11 +928,11 @@
       <c r="AT3" s="6"/>
       <c r="AU3" s="6"/>
       <c r="AV3" s="6"/>
-      <c r="AW3" s="8"/>
+      <c r="AW3" s="6"/>
     </row>
     <row r="4" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="B4" s="11">
         <v>149.24985279121501</v>
@@ -974,7 +972,7 @@
         <f>SUM(H4:L4)</f>
         <v>11.471877574920637</v>
       </c>
-      <c r="N4">
+      <c r="N4" s="11">
         <v>149.24985279121501</v>
       </c>
       <c r="O4">
@@ -989,44 +987,70 @@
       <c r="R4">
         <v>52.527300430865402</v>
       </c>
-      <c r="S4">
+      <c r="S4" s="3">
         <f>SUM(N4:R4)</f>
         <v>647.24140680976484</v>
       </c>
-      <c r="T4" s="2"/>
-      <c r="U4" s="3"/>
-      <c r="V4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="X4" s="3"/>
-      <c r="Y4" s="3"/>
-      <c r="Z4" s="10"/>
+      <c r="T4" s="11">
+        <v>3.0477790355682299</v>
+      </c>
+      <c r="U4">
+        <v>1.4314555168151799</v>
+      </c>
+      <c r="V4">
+        <v>1.74079782962799</v>
+      </c>
+      <c r="W4">
+        <v>3.68662235736846</v>
+      </c>
+      <c r="X4">
+        <v>0.92661826610565101</v>
+      </c>
+      <c r="Y4" s="3">
+        <f>SUM(T4:X4)</f>
+        <v>10.833273005485511</v>
+      </c>
+      <c r="Z4" s="2"/>
       <c r="AA4" s="3"/>
       <c r="AB4" s="3"/>
       <c r="AC4" s="3"/>
       <c r="AD4" s="3"/>
-      <c r="AE4" s="3"/>
+      <c r="AE4" s="5"/>
       <c r="AF4" s="2"/>
       <c r="AG4" s="3"/>
       <c r="AH4" s="3"/>
       <c r="AI4" s="3"/>
       <c r="AJ4" s="3"/>
       <c r="AK4" s="3"/>
-      <c r="AL4" s="2"/>
+      <c r="AL4" s="10"/>
       <c r="AM4" s="3"/>
       <c r="AN4" s="3"/>
       <c r="AO4" s="3"/>
       <c r="AP4" s="3"/>
       <c r="AQ4" s="3"/>
-      <c r="AR4" s="2"/>
-      <c r="AS4" s="3"/>
-      <c r="AT4" s="3"/>
-      <c r="AU4" s="3"/>
-      <c r="AV4" s="3"/>
-      <c r="AW4" s="5"/>
+      <c r="AR4" s="2">
+        <v>149.24985279121501</v>
+      </c>
+      <c r="AS4" s="3">
+        <v>95.799959326746404</v>
+      </c>
+      <c r="AT4" s="3">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AU4" s="3">
+        <v>201.14593791939001</v>
+      </c>
+      <c r="AV4" s="3">
+        <v>52.527300430865402</v>
+      </c>
+      <c r="AW4" s="3">
+        <f>SUM(AR4:AV4)</f>
+        <v>647.24140680976484</v>
+      </c>
     </row>
     <row r="5" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B5" s="2">
         <v>147.69962901947</v>
@@ -1066,11 +1090,11 @@
         <f t="shared" ref="M5:M60" si="1">SUM(H5:L5)</f>
         <v>12.911525774002053</v>
       </c>
-      <c r="N5">
-        <v>147.69962901947</v>
+      <c r="N5" s="2">
+        <v>110.206699026359</v>
       </c>
       <c r="O5">
-        <v>103.66210391121901</v>
+        <v>110.40725555812899</v>
       </c>
       <c r="P5">
         <v>148.51835634154801</v>
@@ -1081,22 +1105,35 @@
       <c r="R5">
         <v>52.527300430865402</v>
       </c>
-      <c r="S5">
-        <f t="shared" ref="S5:S60" si="2">SUM(N5:R5)</f>
-        <v>653.55332762249236</v>
-      </c>
-      <c r="T5" s="2"/>
-      <c r="U5" s="3"/>
-      <c r="V5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="X5" s="3"/>
-      <c r="Y5" s="3"/>
+      <c r="S5" s="3">
+        <f t="shared" ref="S5:S59" si="2">SUM(N5:R5)</f>
+        <v>622.80554927629134</v>
+      </c>
+      <c r="T5" s="2">
+        <v>2.2345791339874199</v>
+      </c>
+      <c r="U5">
+        <v>2.15797202587127</v>
+      </c>
+      <c r="V5">
+        <v>2.3470765352249101</v>
+      </c>
+      <c r="W5">
+        <v>4.2425618410110397</v>
+      </c>
+      <c r="X5">
+        <v>0.81414456367492605</v>
+      </c>
+      <c r="Y5" s="3">
+        <f t="shared" ref="Y5:Y59" si="3">SUM(T5:X5)</f>
+        <v>11.796334099769567</v>
+      </c>
       <c r="Z5" s="2"/>
       <c r="AA5" s="3"/>
       <c r="AB5" s="3"/>
       <c r="AC5" s="3"/>
       <c r="AD5" s="3"/>
-      <c r="AE5" s="3"/>
+      <c r="AE5" s="5"/>
       <c r="AF5" s="2"/>
       <c r="AG5" s="3"/>
       <c r="AH5" s="3"/>
@@ -1109,16 +1146,29 @@
       <c r="AO5" s="3"/>
       <c r="AP5" s="3"/>
       <c r="AQ5" s="3"/>
-      <c r="AR5" s="2"/>
-      <c r="AS5" s="3"/>
-      <c r="AT5" s="3"/>
-      <c r="AU5" s="3"/>
-      <c r="AV5" s="3"/>
-      <c r="AW5" s="5"/>
+      <c r="AR5" s="2">
+        <v>147.69962901947</v>
+      </c>
+      <c r="AS5" s="3">
+        <v>103.66210391121901</v>
+      </c>
+      <c r="AT5" s="3">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AU5" s="3">
+        <v>201.14593791939001</v>
+      </c>
+      <c r="AV5" s="3">
+        <v>52.527300430865402</v>
+      </c>
+      <c r="AW5" s="3">
+        <f t="shared" ref="AW5:AW60" si="4">SUM(AR5:AV5)</f>
+        <v>653.55332762249236</v>
+      </c>
     </row>
     <row r="6" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="B6" s="2">
         <v>151.11957368607401</v>
@@ -1158,7 +1208,7 @@
         <f t="shared" si="1"/>
         <v>16.204109764099101</v>
       </c>
-      <c r="N6">
+      <c r="N6" s="2">
         <v>151.11957368607401</v>
       </c>
       <c r="O6">
@@ -1173,22 +1223,35 @@
       <c r="R6">
         <v>109.76092543441101</v>
       </c>
-      <c r="S6">
+      <c r="S6" s="3">
         <f t="shared" si="2"/>
         <v>702.36985449069584</v>
       </c>
-      <c r="T6" s="2"/>
-      <c r="U6" s="3"/>
-      <c r="V6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="X6" s="3"/>
-      <c r="Y6" s="3"/>
+      <c r="T6" s="2">
+        <v>3.8143922328948898</v>
+      </c>
+      <c r="U6">
+        <v>1.82517144680023</v>
+      </c>
+      <c r="V6">
+        <v>2.8470872402191101</v>
+      </c>
+      <c r="W6">
+        <v>5.9051944255828799</v>
+      </c>
+      <c r="X6">
+        <v>0.90319273471832195</v>
+      </c>
+      <c r="Y6" s="3">
+        <f t="shared" si="3"/>
+        <v>15.295038080215432</v>
+      </c>
       <c r="Z6" s="2"/>
       <c r="AA6" s="3"/>
       <c r="AB6" s="3"/>
       <c r="AC6" s="3"/>
       <c r="AD6" s="3"/>
-      <c r="AE6" s="3"/>
+      <c r="AE6" s="5"/>
       <c r="AF6" s="2"/>
       <c r="AG6" s="3"/>
       <c r="AH6" s="3"/>
@@ -1201,16 +1264,29 @@
       <c r="AO6" s="3"/>
       <c r="AP6" s="3"/>
       <c r="AQ6" s="3"/>
-      <c r="AR6" s="2"/>
-      <c r="AS6" s="3"/>
-      <c r="AT6" s="3"/>
-      <c r="AU6" s="3"/>
-      <c r="AV6" s="3"/>
-      <c r="AW6" s="5"/>
+      <c r="AR6" s="2">
+        <v>151.11957368607401</v>
+      </c>
+      <c r="AS6" s="3">
+        <v>93.360450951570897</v>
+      </c>
+      <c r="AT6" s="3">
+        <v>147.73999534465699</v>
+      </c>
+      <c r="AU6" s="3">
+        <v>200.388909073983</v>
+      </c>
+      <c r="AV6" s="3">
+        <v>109.76092543441101</v>
+      </c>
+      <c r="AW6" s="3">
+        <f t="shared" si="4"/>
+        <v>702.36985449069584</v>
+      </c>
     </row>
     <row r="7" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="B7" s="2">
         <v>188.76575923012899</v>
@@ -1250,37 +1326,50 @@
         <f>SUM(H7:L7)</f>
         <v>27.59067518711079</v>
       </c>
-      <c r="N7">
-        <v>188.76575923012899</v>
+      <c r="N7" s="2">
+        <v>159.149154352317</v>
       </c>
       <c r="O7">
-        <v>106.78060331663001</v>
+        <v>108.96970109297401</v>
       </c>
       <c r="P7">
-        <v>130.862087378181</v>
+        <v>144.47355668633099</v>
       </c>
       <c r="Q7">
-        <v>194.79950731981299</v>
+        <v>194.93208222335599</v>
       </c>
       <c r="R7">
         <v>109.76092543441101</v>
       </c>
-      <c r="S7">
-        <f>SUM(N7:R7)</f>
-        <v>730.96888267916393</v>
-      </c>
-      <c r="T7" s="2"/>
-      <c r="U7" s="3"/>
-      <c r="V7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="3"/>
+      <c r="S7" s="3">
+        <f t="shared" si="2"/>
+        <v>717.28541978938892</v>
+      </c>
+      <c r="T7" s="2">
+        <v>6.2202388763427701</v>
+      </c>
+      <c r="U7">
+        <v>2.3331806182861299</v>
+      </c>
+      <c r="V7">
+        <v>4.2638045072555499</v>
+      </c>
+      <c r="W7">
+        <v>10.3235799074172</v>
+      </c>
+      <c r="X7">
+        <v>1.2231767654418899</v>
+      </c>
+      <c r="Y7" s="3">
+        <f t="shared" si="3"/>
+        <v>24.363980674743537</v>
+      </c>
       <c r="Z7" s="2"/>
       <c r="AA7" s="3"/>
       <c r="AB7" s="3"/>
       <c r="AC7" s="3"/>
       <c r="AD7" s="3"/>
-      <c r="AE7" s="3"/>
+      <c r="AE7" s="5"/>
       <c r="AF7" s="2"/>
       <c r="AG7" s="3"/>
       <c r="AH7" s="3"/>
@@ -1293,16 +1382,29 @@
       <c r="AO7" s="3"/>
       <c r="AP7" s="3"/>
       <c r="AQ7" s="3"/>
-      <c r="AR7" s="2"/>
-      <c r="AS7" s="3"/>
-      <c r="AT7" s="3"/>
-      <c r="AU7" s="3"/>
-      <c r="AV7" s="3"/>
-      <c r="AW7" s="5"/>
+      <c r="AR7" s="2">
+        <v>188.76575923012899</v>
+      </c>
+      <c r="AS7" s="3">
+        <v>106.78060331663001</v>
+      </c>
+      <c r="AT7" s="3">
+        <v>130.862087378181</v>
+      </c>
+      <c r="AU7" s="3">
+        <v>194.79950731981299</v>
+      </c>
+      <c r="AV7" s="3">
+        <v>109.76092543441101</v>
+      </c>
+      <c r="AW7" s="3">
+        <f>SUM(AR7:AV7)</f>
+        <v>730.96888267916393</v>
+      </c>
     </row>
     <row r="8" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B8" s="2">
         <v>148.756384553087</v>
@@ -1342,11 +1444,11 @@
         <f>SUM(H8:L8)</f>
         <v>11.662139773368825</v>
       </c>
-      <c r="N8">
-        <v>148.756384553087</v>
+      <c r="N8" s="2">
+        <v>110.206699026359</v>
       </c>
       <c r="O8">
-        <v>98.782327103466301</v>
+        <v>110.75770598915599</v>
       </c>
       <c r="P8">
         <v>148.51835634154801</v>
@@ -1357,22 +1459,35 @@
       <c r="R8">
         <v>52.527300430865402</v>
       </c>
-      <c r="S8">
+      <c r="S8" s="3">
         <f t="shared" si="2"/>
-        <v>646.54281853988959</v>
-      </c>
-      <c r="T8" s="2"/>
-      <c r="U8" s="3"/>
-      <c r="V8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="3"/>
+        <v>619.96851189885138</v>
+      </c>
+      <c r="T8" s="2">
+        <v>2.4033009052276602</v>
+      </c>
+      <c r="U8">
+        <v>1.71264998912811</v>
+      </c>
+      <c r="V8">
+        <v>1.7939531564712501</v>
+      </c>
+      <c r="W8">
+        <v>3.7206792354583702</v>
+      </c>
+      <c r="X8">
+        <v>0.85791544914245599</v>
+      </c>
+      <c r="Y8" s="3">
+        <f t="shared" si="3"/>
+        <v>10.488498735427846</v>
+      </c>
       <c r="Z8" s="2"/>
       <c r="AA8" s="3"/>
       <c r="AB8" s="3"/>
       <c r="AC8" s="3"/>
       <c r="AD8" s="3"/>
-      <c r="AE8" s="3"/>
+      <c r="AE8" s="5"/>
       <c r="AF8" s="2"/>
       <c r="AG8" s="3"/>
       <c r="AH8" s="3"/>
@@ -1385,16 +1500,29 @@
       <c r="AO8" s="3"/>
       <c r="AP8" s="3"/>
       <c r="AQ8" s="3"/>
-      <c r="AR8" s="2"/>
-      <c r="AS8" s="3"/>
-      <c r="AT8" s="3"/>
-      <c r="AU8" s="3"/>
-      <c r="AV8" s="3"/>
-      <c r="AW8" s="5"/>
+      <c r="AR8" s="2">
+        <v>148.756384553087</v>
+      </c>
+      <c r="AS8" s="3">
+        <v>98.782327103466301</v>
+      </c>
+      <c r="AT8" s="3">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AU8" s="3">
+        <v>197.958450110923</v>
+      </c>
+      <c r="AV8" s="3">
+        <v>52.527300430865402</v>
+      </c>
+      <c r="AW8" s="3">
+        <f t="shared" si="4"/>
+        <v>646.54281853988959</v>
+      </c>
     </row>
     <row r="9" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B9" s="2">
         <v>210.31133459479599</v>
@@ -1434,14 +1562,14 @@
         <f t="shared" si="1"/>
         <v>12.68032891750333</v>
       </c>
-      <c r="N9">
-        <v>210.31133459479599</v>
+      <c r="N9" s="2">
+        <v>110.206699026359</v>
       </c>
       <c r="O9">
-        <v>97.913145460499507</v>
+        <v>110.75770598915599</v>
       </c>
       <c r="P9">
-        <v>139.45006854101001</v>
+        <v>148.51835634154801</v>
       </c>
       <c r="Q9">
         <v>201.14593791939001</v>
@@ -1449,22 +1577,35 @@
       <c r="R9">
         <v>52.527300430865402</v>
       </c>
-      <c r="S9">
+      <c r="S9" s="3">
         <f t="shared" si="2"/>
-        <v>701.34778694656086</v>
-      </c>
-      <c r="T9" s="2"/>
-      <c r="U9" s="3"/>
-      <c r="V9" s="3"/>
-      <c r="W9" s="3"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="3"/>
+        <v>623.15599970731841</v>
+      </c>
+      <c r="T9" s="2">
+        <v>2.3393565177917401</v>
+      </c>
+      <c r="U9">
+        <v>1.7205018281936599</v>
+      </c>
+      <c r="V9">
+        <v>2.2440066576004001</v>
+      </c>
+      <c r="W9">
+        <v>3.80350637435913</v>
+      </c>
+      <c r="X9">
+        <v>1.01592309474945</v>
+      </c>
+      <c r="Y9" s="3">
+        <f t="shared" si="3"/>
+        <v>11.123294472694379</v>
+      </c>
       <c r="Z9" s="2"/>
       <c r="AA9" s="3"/>
       <c r="AB9" s="3"/>
       <c r="AC9" s="3"/>
       <c r="AD9" s="3"/>
-      <c r="AE9" s="3"/>
+      <c r="AE9" s="5"/>
       <c r="AF9" s="2"/>
       <c r="AG9" s="3"/>
       <c r="AH9" s="3"/>
@@ -1477,16 +1618,29 @@
       <c r="AO9" s="3"/>
       <c r="AP9" s="3"/>
       <c r="AQ9" s="3"/>
-      <c r="AR9" s="2"/>
-      <c r="AS9" s="3"/>
-      <c r="AT9" s="3"/>
-      <c r="AU9" s="3"/>
-      <c r="AV9" s="3"/>
-      <c r="AW9" s="5"/>
+      <c r="AR9" s="2">
+        <v>210.31133459479599</v>
+      </c>
+      <c r="AS9" s="3">
+        <v>97.913145460499507</v>
+      </c>
+      <c r="AT9" s="3">
+        <v>139.45006854101001</v>
+      </c>
+      <c r="AU9" s="3">
+        <v>201.14593791939001</v>
+      </c>
+      <c r="AV9" s="3">
+        <v>52.527300430865402</v>
+      </c>
+      <c r="AW9" s="3">
+        <f t="shared" si="4"/>
+        <v>701.34778694656086</v>
+      </c>
     </row>
     <row r="10" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B10" s="2">
         <v>147.69962901947</v>
@@ -1526,11 +1680,11 @@
         <f t="shared" si="1"/>
         <v>11.848121118545526</v>
       </c>
-      <c r="N10">
-        <v>147.69962901947</v>
+      <c r="N10" s="2">
+        <v>156.21310732000299</v>
       </c>
       <c r="O10">
-        <v>103.760923458101</v>
+        <v>106.466545429337</v>
       </c>
       <c r="P10">
         <v>148.51835634154801</v>
@@ -1541,22 +1695,35 @@
       <c r="R10">
         <v>52.527300430865402</v>
       </c>
-      <c r="S10">
+      <c r="S10" s="3">
         <f t="shared" si="2"/>
-        <v>653.65214716937442</v>
-      </c>
-      <c r="T10" s="2"/>
-      <c r="U10" s="3"/>
-      <c r="V10" s="3"/>
-      <c r="W10" s="3"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="3"/>
+        <v>664.8712474411434</v>
+      </c>
+      <c r="T10" s="2">
+        <v>2.9830847978591901</v>
+      </c>
+      <c r="U10">
+        <v>1.6767358303069999</v>
+      </c>
+      <c r="V10">
+        <v>1.8814272880554199</v>
+      </c>
+      <c r="W10">
+        <v>3.75041236877441</v>
+      </c>
+      <c r="X10">
+        <v>0.85629050731658896</v>
+      </c>
+      <c r="Y10" s="3">
+        <f t="shared" si="3"/>
+        <v>11.147950792312608</v>
+      </c>
       <c r="Z10" s="2"/>
       <c r="AA10" s="3"/>
       <c r="AB10" s="3"/>
       <c r="AC10" s="3"/>
       <c r="AD10" s="3"/>
-      <c r="AE10" s="3"/>
+      <c r="AE10" s="5"/>
       <c r="AF10" s="2"/>
       <c r="AG10" s="3"/>
       <c r="AH10" s="3"/>
@@ -1569,16 +1736,29 @@
       <c r="AO10" s="3"/>
       <c r="AP10" s="3"/>
       <c r="AQ10" s="3"/>
-      <c r="AR10" s="2"/>
-      <c r="AS10" s="3"/>
-      <c r="AT10" s="3"/>
-      <c r="AU10" s="3"/>
-      <c r="AV10" s="3"/>
-      <c r="AW10" s="5"/>
+      <c r="AR10" s="2">
+        <v>147.69962901947</v>
+      </c>
+      <c r="AS10" s="3">
+        <v>103.760923458101</v>
+      </c>
+      <c r="AT10" s="3">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AU10" s="3">
+        <v>201.14593791939001</v>
+      </c>
+      <c r="AV10" s="3">
+        <v>52.527300430865402</v>
+      </c>
+      <c r="AW10" s="3">
+        <f t="shared" si="4"/>
+        <v>653.65214716937442</v>
+      </c>
     </row>
     <row r="11" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B11" s="2">
         <v>151.98178517246799</v>
@@ -1618,7 +1798,7 @@
         <f t="shared" si="1"/>
         <v>14.955296397209141</v>
       </c>
-      <c r="N11">
+      <c r="N11" s="2">
         <v>151.98178517246799</v>
       </c>
       <c r="O11">
@@ -1628,27 +1808,40 @@
         <v>148.51835634154801</v>
       </c>
       <c r="Q11">
-        <v>201.212942557161</v>
+        <v>201.14593791939001</v>
       </c>
       <c r="R11">
         <v>52.527300430865402</v>
       </c>
-      <c r="S11">
+      <c r="S11" s="3">
         <f t="shared" si="2"/>
-        <v>650.83011734306001</v>
-      </c>
-      <c r="T11" s="2"/>
-      <c r="U11" s="3"/>
-      <c r="V11" s="3"/>
-      <c r="W11" s="3"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="3"/>
+        <v>650.7631127052889</v>
+      </c>
+      <c r="T11" s="2">
+        <v>3.82228293418884</v>
+      </c>
+      <c r="U11">
+        <v>1.6205398321151701</v>
+      </c>
+      <c r="V11">
+        <v>2.1908255100250198</v>
+      </c>
+      <c r="W11">
+        <v>4.7067322492599404</v>
+      </c>
+      <c r="X11">
+        <v>1.05007333755493</v>
+      </c>
+      <c r="Y11" s="3">
+        <f t="shared" si="3"/>
+        <v>13.3904538631439</v>
+      </c>
       <c r="Z11" s="2"/>
       <c r="AA11" s="3"/>
       <c r="AB11" s="3"/>
       <c r="AC11" s="3"/>
       <c r="AD11" s="3"/>
-      <c r="AE11" s="3"/>
+      <c r="AE11" s="5"/>
       <c r="AF11" s="2"/>
       <c r="AG11" s="3"/>
       <c r="AH11" s="3"/>
@@ -1661,16 +1854,29 @@
       <c r="AO11" s="3"/>
       <c r="AP11" s="3"/>
       <c r="AQ11" s="3"/>
-      <c r="AR11" s="2"/>
-      <c r="AS11" s="3"/>
-      <c r="AT11" s="3"/>
-      <c r="AU11" s="3"/>
-      <c r="AV11" s="3"/>
-      <c r="AW11" s="5"/>
+      <c r="AR11" s="2">
+        <v>151.98178517246799</v>
+      </c>
+      <c r="AS11" s="3">
+        <v>96.589732841017593</v>
+      </c>
+      <c r="AT11" s="3">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AU11" s="3">
+        <v>201.212942557161</v>
+      </c>
+      <c r="AV11" s="3">
+        <v>52.527300430865402</v>
+      </c>
+      <c r="AW11" s="3">
+        <f t="shared" si="4"/>
+        <v>650.83011734306001</v>
+      </c>
     </row>
     <row r="12" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B12" s="2">
         <v>150.81021229721401</v>
@@ -1710,11 +1916,11 @@
         <f t="shared" si="1"/>
         <v>20.366134023666362</v>
       </c>
-      <c r="N12">
-        <v>150.81021229721401</v>
+      <c r="N12" s="2">
+        <v>166.22175006309999</v>
       </c>
       <c r="O12">
-        <v>91.380348344503801</v>
+        <v>71.823998382771094</v>
       </c>
       <c r="P12">
         <v>148.51835634154801</v>
@@ -1723,24 +1929,37 @@
         <v>201.14593791939001</v>
       </c>
       <c r="R12">
-        <v>97.6493571215793</v>
-      </c>
-      <c r="S12">
+        <v>52.527300430865402</v>
+      </c>
+      <c r="S12" s="3">
         <f t="shared" si="2"/>
-        <v>689.50421202423513</v>
-      </c>
-      <c r="T12" s="2"/>
-      <c r="U12" s="3"/>
-      <c r="V12" s="3"/>
-      <c r="W12" s="3"/>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="3"/>
+        <v>640.23734313767443</v>
+      </c>
+      <c r="T12" s="2">
+        <v>9.6007839441299403</v>
+      </c>
+      <c r="U12">
+        <v>0.97194740772247301</v>
+      </c>
+      <c r="V12">
+        <v>3.7049924850463798</v>
+      </c>
+      <c r="W12">
+        <v>6.4770827054977396</v>
+      </c>
+      <c r="X12">
+        <v>1.13138213157653</v>
+      </c>
+      <c r="Y12" s="3">
+        <f t="shared" si="3"/>
+        <v>21.886188673973063</v>
+      </c>
       <c r="Z12" s="2"/>
       <c r="AA12" s="3"/>
       <c r="AB12" s="3"/>
       <c r="AC12" s="3"/>
       <c r="AD12" s="3"/>
-      <c r="AE12" s="3"/>
+      <c r="AE12" s="5"/>
       <c r="AF12" s="2"/>
       <c r="AG12" s="3"/>
       <c r="AH12" s="3"/>
@@ -1753,18 +1972,31 @@
       <c r="AO12" s="3"/>
       <c r="AP12" s="3"/>
       <c r="AQ12" s="3"/>
-      <c r="AR12" s="2"/>
-      <c r="AS12" s="3"/>
-      <c r="AT12" s="3"/>
-      <c r="AU12" s="3"/>
-      <c r="AV12" s="3"/>
-      <c r="AW12" s="5"/>
+      <c r="AR12" s="2">
+        <v>150.81021229721401</v>
+      </c>
+      <c r="AS12" s="3">
+        <v>91.380348344503801</v>
+      </c>
+      <c r="AT12" s="3">
+        <v>148.51835634154801</v>
+      </c>
+      <c r="AU12" s="3">
+        <v>201.14593791939001</v>
+      </c>
+      <c r="AV12" s="3">
+        <v>97.6493571215793</v>
+      </c>
+      <c r="AW12" s="3">
+        <f t="shared" si="4"/>
+        <v>689.50421202423513</v>
+      </c>
     </row>
     <row r="13" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>18</v>
-      </c>
-      <c r="B13">
+        <v>16</v>
+      </c>
+      <c r="B13" s="2">
         <v>247.216798456151</v>
       </c>
       <c r="C13">
@@ -1802,22 +2034,50 @@
         <f t="shared" si="1"/>
         <v>11.96596469879149</v>
       </c>
-      <c r="S13">
+      <c r="N13" s="2">
+        <v>251.68529934636101</v>
+      </c>
+      <c r="O13">
+        <v>152.765610009699</v>
+      </c>
+      <c r="P13">
+        <v>238.63534163309501</v>
+      </c>
+      <c r="Q13">
+        <v>255.51866651167501</v>
+      </c>
+      <c r="R13">
+        <v>109.154249735316</v>
+      </c>
+      <c r="S13" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T13" s="2"/>
-      <c r="U13" s="3"/>
-      <c r="V13" s="3"/>
-      <c r="W13" s="3"/>
-      <c r="X13" s="3"/>
-      <c r="Y13" s="3"/>
+        <v>1007.7591672361459</v>
+      </c>
+      <c r="T13" s="2">
+        <v>2.26439931392669</v>
+      </c>
+      <c r="U13">
+        <v>1.73920748233795</v>
+      </c>
+      <c r="V13">
+        <v>2.95509502887725</v>
+      </c>
+      <c r="W13">
+        <v>4.9817697048187197</v>
+      </c>
+      <c r="X13">
+        <v>0.51254746913909899</v>
+      </c>
+      <c r="Y13" s="3">
+        <f t="shared" si="3"/>
+        <v>12.453018999099708</v>
+      </c>
       <c r="Z13" s="2"/>
       <c r="AA13" s="3"/>
       <c r="AB13" s="3"/>
       <c r="AC13" s="3"/>
       <c r="AD13" s="3"/>
-      <c r="AE13" s="3"/>
+      <c r="AE13" s="5"/>
       <c r="AF13" s="2"/>
       <c r="AG13" s="3"/>
       <c r="AH13" s="3"/>
@@ -1831,17 +2091,16 @@
       <c r="AP13" s="3"/>
       <c r="AQ13" s="3"/>
       <c r="AR13" s="2"/>
-      <c r="AS13" s="3"/>
-      <c r="AT13" s="3"/>
-      <c r="AU13" s="3"/>
-      <c r="AV13" s="3"/>
-      <c r="AW13" s="5"/>
+      <c r="AW13">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="14" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>19</v>
-      </c>
-      <c r="B14">
+        <v>17</v>
+      </c>
+      <c r="B14" s="2">
         <v>249.329909798448</v>
       </c>
       <c r="C14">
@@ -1879,22 +2138,50 @@
         <f t="shared" si="1"/>
         <v>23.054575061798072</v>
       </c>
-      <c r="S14">
+      <c r="N14" s="2">
+        <v>355.25666964872499</v>
+      </c>
+      <c r="O14">
+        <v>169.55286584768399</v>
+      </c>
+      <c r="P14">
+        <v>175.027007071204</v>
+      </c>
+      <c r="Q14">
+        <v>271.58371380737401</v>
+      </c>
+      <c r="R14">
+        <v>170.677305023836</v>
+      </c>
+      <c r="S14" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T14" s="2"/>
-      <c r="U14" s="3"/>
-      <c r="V14" s="3"/>
-      <c r="W14" s="3"/>
-      <c r="X14" s="3"/>
-      <c r="Y14" s="3"/>
+        <v>1142.097561398823</v>
+      </c>
+      <c r="T14" s="2">
+        <v>6.3681014060974102</v>
+      </c>
+      <c r="U14">
+        <v>1.6659356117248501</v>
+      </c>
+      <c r="V14">
+        <v>2.5593135595321601</v>
+      </c>
+      <c r="W14">
+        <v>4.79603767395019</v>
+      </c>
+      <c r="X14">
+        <v>2.40033922195434</v>
+      </c>
+      <c r="Y14" s="3">
+        <f t="shared" si="3"/>
+        <v>17.789727473258949</v>
+      </c>
       <c r="Z14" s="2"/>
       <c r="AA14" s="3"/>
       <c r="AB14" s="3"/>
       <c r="AC14" s="3"/>
       <c r="AD14" s="3"/>
-      <c r="AE14" s="3"/>
+      <c r="AE14" s="5"/>
       <c r="AF14" s="2"/>
       <c r="AG14" s="3"/>
       <c r="AH14" s="3"/>
@@ -1908,17 +2195,16 @@
       <c r="AP14" s="3"/>
       <c r="AQ14" s="3"/>
       <c r="AR14" s="2"/>
-      <c r="AS14" s="3"/>
-      <c r="AT14" s="3"/>
-      <c r="AU14" s="3"/>
-      <c r="AV14" s="3"/>
-      <c r="AW14" s="5"/>
+      <c r="AW14">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="15" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>20</v>
-      </c>
-      <c r="B15">
+        <v>18</v>
+      </c>
+      <c r="B15" s="2">
         <v>232.82055388303499</v>
       </c>
       <c r="C15">
@@ -1956,22 +2242,50 @@
         <f t="shared" si="1"/>
         <v>35.024655866622787</v>
       </c>
-      <c r="S15">
+      <c r="N15" s="2">
+        <v>248.386676946763</v>
+      </c>
+      <c r="O15">
+        <v>179.98771894786299</v>
+      </c>
+      <c r="P15">
+        <v>169.836294051935</v>
+      </c>
+      <c r="Q15">
+        <v>260.23007768031903</v>
+      </c>
+      <c r="R15">
+        <v>168.49066569943801</v>
+      </c>
+      <c r="S15" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T15" s="2"/>
-      <c r="U15" s="3"/>
-      <c r="V15" s="3"/>
-      <c r="W15" s="3"/>
-      <c r="X15" s="3"/>
-      <c r="Y15" s="3"/>
+        <v>1026.931433326318</v>
+      </c>
+      <c r="T15" s="2">
+        <v>2.2064824104309002</v>
+      </c>
+      <c r="U15">
+        <v>7.9181566715240397</v>
+      </c>
+      <c r="V15">
+        <v>3.1550543308257999</v>
+      </c>
+      <c r="W15">
+        <v>16.292787027359001</v>
+      </c>
+      <c r="X15">
+        <v>3.4363976240157998</v>
+      </c>
+      <c r="Y15" s="3">
+        <f t="shared" si="3"/>
+        <v>33.008878064155539</v>
+      </c>
       <c r="Z15" s="2"/>
       <c r="AA15" s="3"/>
       <c r="AB15" s="3"/>
       <c r="AC15" s="3"/>
       <c r="AD15" s="3"/>
-      <c r="AE15" s="3"/>
+      <c r="AE15" s="5"/>
       <c r="AF15" s="2"/>
       <c r="AG15" s="3"/>
       <c r="AH15" s="3"/>
@@ -1985,17 +2299,16 @@
       <c r="AP15" s="3"/>
       <c r="AQ15" s="3"/>
       <c r="AR15" s="2"/>
-      <c r="AS15" s="3"/>
-      <c r="AT15" s="3"/>
-      <c r="AU15" s="3"/>
-      <c r="AV15" s="3"/>
-      <c r="AW15" s="5"/>
+      <c r="AW15">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="16" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>21</v>
-      </c>
-      <c r="B16">
+        <v>19</v>
+      </c>
+      <c r="B16" s="2">
         <v>236.205554831212</v>
       </c>
       <c r="C16">
@@ -2033,22 +2346,50 @@
         <f t="shared" si="1"/>
         <v>80.302021074295013</v>
       </c>
-      <c r="S16">
+      <c r="N16" s="2">
+        <v>227.55330022553099</v>
+      </c>
+      <c r="O16">
+        <v>151.758552352408</v>
+      </c>
+      <c r="P16">
+        <v>170.90320200033699</v>
+      </c>
+      <c r="Q16">
+        <v>255.33792632727699</v>
+      </c>
+      <c r="R16">
+        <v>157.00160565636</v>
+      </c>
+      <c r="S16" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T16" s="2"/>
-      <c r="U16" s="3"/>
-      <c r="V16" s="3"/>
-      <c r="W16" s="3"/>
-      <c r="X16" s="3"/>
-      <c r="Y16" s="3"/>
+        <v>962.55458656191308</v>
+      </c>
+      <c r="T16" s="2">
+        <v>5.2925606727599996</v>
+      </c>
+      <c r="U16">
+        <v>5.37200829982757</v>
+      </c>
+      <c r="V16">
+        <v>3.7663801193237298</v>
+      </c>
+      <c r="W16">
+        <v>49.691688394546503</v>
+      </c>
+      <c r="X16">
+        <v>4.5744156122207604</v>
+      </c>
+      <c r="Y16" s="3">
+        <f t="shared" si="3"/>
+        <v>68.697053098678566</v>
+      </c>
       <c r="Z16" s="2"/>
       <c r="AA16" s="3"/>
       <c r="AB16" s="3"/>
       <c r="AC16" s="3"/>
       <c r="AD16" s="3"/>
-      <c r="AE16" s="3"/>
+      <c r="AE16" s="5"/>
       <c r="AF16" s="2"/>
       <c r="AG16" s="3"/>
       <c r="AH16" s="3"/>
@@ -2062,17 +2403,16 @@
       <c r="AP16" s="3"/>
       <c r="AQ16" s="3"/>
       <c r="AR16" s="2"/>
-      <c r="AS16" s="3"/>
-      <c r="AT16" s="3"/>
-      <c r="AU16" s="3"/>
-      <c r="AV16" s="3"/>
-      <c r="AW16" s="5"/>
+      <c r="AW16">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>22</v>
-      </c>
-      <c r="B17">
+        <v>20</v>
+      </c>
+      <c r="B17" s="2">
         <v>289.62720165852699</v>
       </c>
       <c r="C17">
@@ -2110,22 +2450,50 @@
         <f t="shared" si="1"/>
         <v>17.97586321830747</v>
       </c>
-      <c r="S17">
+      <c r="N17" s="2">
+        <v>313.13217148424201</v>
+      </c>
+      <c r="O17">
+        <v>153.274802852101</v>
+      </c>
+      <c r="P17">
+        <v>241.67154979377401</v>
+      </c>
+      <c r="Q17">
+        <v>186.905239211657</v>
+      </c>
+      <c r="R17">
+        <v>115.566897157905</v>
+      </c>
+      <c r="S17" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T17" s="2"/>
-      <c r="U17" s="3"/>
-      <c r="V17" s="3"/>
-      <c r="W17" s="3"/>
-      <c r="X17" s="3"/>
-      <c r="Y17" s="3"/>
+        <v>1010.550660499679</v>
+      </c>
+      <c r="T17" s="2">
+        <v>4.3209599018096903</v>
+      </c>
+      <c r="U17">
+        <v>3.8848403692245399</v>
+      </c>
+      <c r="V17">
+        <v>5.3037979125976502</v>
+      </c>
+      <c r="W17">
+        <v>4.2083729982376097</v>
+      </c>
+      <c r="X17">
+        <v>1.0704200029373101</v>
+      </c>
+      <c r="Y17" s="3">
+        <f t="shared" si="3"/>
+        <v>18.788391184806802</v>
+      </c>
       <c r="Z17" s="2"/>
       <c r="AA17" s="3"/>
       <c r="AB17" s="3"/>
       <c r="AC17" s="3"/>
       <c r="AD17" s="3"/>
-      <c r="AE17" s="3"/>
+      <c r="AE17" s="5"/>
       <c r="AF17" s="2"/>
       <c r="AG17" s="3"/>
       <c r="AH17" s="3"/>
@@ -2139,17 +2507,16 @@
       <c r="AP17" s="3"/>
       <c r="AQ17" s="3"/>
       <c r="AR17" s="2"/>
-      <c r="AS17" s="3"/>
-      <c r="AT17" s="3"/>
-      <c r="AU17" s="3"/>
-      <c r="AV17" s="3"/>
-      <c r="AW17" s="5"/>
+      <c r="AW17">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="18" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B18">
+        <v>21</v>
+      </c>
+      <c r="B18" s="2">
         <v>274.06888138866702</v>
       </c>
       <c r="C18">
@@ -2187,22 +2554,50 @@
         <f t="shared" si="1"/>
         <v>28.045329022407483</v>
       </c>
-      <c r="S18">
+      <c r="N18" s="2">
+        <v>133.592581412154</v>
+      </c>
+      <c r="O18">
+        <v>151.692810330192</v>
+      </c>
+      <c r="P18">
+        <v>255.510506326995</v>
+      </c>
+      <c r="Q18">
+        <v>280.96764744164699</v>
+      </c>
+      <c r="R18">
+        <v>71.054083775364404</v>
+      </c>
+      <c r="S18" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T18" s="2"/>
-      <c r="U18" s="3"/>
-      <c r="V18" s="3"/>
-      <c r="W18" s="3"/>
-      <c r="X18" s="3"/>
-      <c r="Y18" s="3"/>
+        <v>892.81762928635248</v>
+      </c>
+      <c r="T18" s="2">
+        <v>1.4330073118209801</v>
+      </c>
+      <c r="U18">
+        <v>2.5986635446548401</v>
+      </c>
+      <c r="V18">
+        <v>12.1140716075897</v>
+      </c>
+      <c r="W18">
+        <v>16.128396844863801</v>
+      </c>
+      <c r="X18">
+        <v>0.42658348083496</v>
+      </c>
+      <c r="Y18" s="3">
+        <f t="shared" si="3"/>
+        <v>32.700722789764278</v>
+      </c>
       <c r="Z18" s="2"/>
       <c r="AA18" s="3"/>
       <c r="AB18" s="3"/>
       <c r="AC18" s="3"/>
       <c r="AD18" s="3"/>
-      <c r="AE18" s="3"/>
+      <c r="AE18" s="5"/>
       <c r="AF18" s="2"/>
       <c r="AG18" s="3"/>
       <c r="AH18" s="3"/>
@@ -2216,17 +2611,16 @@
       <c r="AP18" s="3"/>
       <c r="AQ18" s="3"/>
       <c r="AR18" s="2"/>
-      <c r="AS18" s="3"/>
-      <c r="AT18" s="3"/>
-      <c r="AU18" s="3"/>
-      <c r="AV18" s="3"/>
-      <c r="AW18" s="5"/>
+      <c r="AW18">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="19" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>24</v>
-      </c>
-      <c r="B19">
+        <v>22</v>
+      </c>
+      <c r="B19" s="2">
         <v>289.62720165852699</v>
       </c>
       <c r="C19">
@@ -2264,22 +2658,50 @@
         <f t="shared" si="1"/>
         <v>27.130878233909531</v>
       </c>
-      <c r="S19">
+      <c r="N19" s="2">
+        <v>238.59251491518901</v>
+      </c>
+      <c r="O19">
+        <v>153.06827551576001</v>
+      </c>
+      <c r="P19">
+        <v>241.723470577923</v>
+      </c>
+      <c r="Q19">
+        <v>217.005114020337</v>
+      </c>
+      <c r="R19">
+        <v>115.566897157905</v>
+      </c>
+      <c r="S19" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T19" s="2"/>
-      <c r="U19" s="3"/>
-      <c r="V19" s="3"/>
-      <c r="W19" s="3"/>
-      <c r="X19" s="3"/>
-      <c r="Y19" s="3"/>
+        <v>965.95627218711411</v>
+      </c>
+      <c r="T19" s="2">
+        <v>3.1300533294677702</v>
+      </c>
+      <c r="U19">
+        <v>9.7012171506881693</v>
+      </c>
+      <c r="V19">
+        <v>3.9551511049270598</v>
+      </c>
+      <c r="W19">
+        <v>11.0763450145721</v>
+      </c>
+      <c r="X19">
+        <v>1.2469570636749201</v>
+      </c>
+      <c r="Y19" s="3">
+        <f t="shared" si="3"/>
+        <v>29.109723663330016</v>
+      </c>
       <c r="Z19" s="2"/>
       <c r="AA19" s="3"/>
       <c r="AB19" s="3"/>
       <c r="AC19" s="3"/>
       <c r="AD19" s="3"/>
-      <c r="AE19" s="3"/>
+      <c r="AE19" s="5"/>
       <c r="AF19" s="2"/>
       <c r="AG19" s="3"/>
       <c r="AH19" s="3"/>
@@ -2293,17 +2715,16 @@
       <c r="AP19" s="3"/>
       <c r="AQ19" s="3"/>
       <c r="AR19" s="2"/>
-      <c r="AS19" s="3"/>
-      <c r="AT19" s="3"/>
-      <c r="AU19" s="3"/>
-      <c r="AV19" s="3"/>
-      <c r="AW19" s="5"/>
+      <c r="AW19">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="20" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>25</v>
-      </c>
-      <c r="B20">
+        <v>23</v>
+      </c>
+      <c r="B20" s="2">
         <v>289.389614297013</v>
       </c>
       <c r="C20">
@@ -2341,22 +2762,50 @@
         <f t="shared" si="1"/>
         <v>25.219599413871737</v>
       </c>
-      <c r="S20">
+      <c r="N20" s="2">
+        <v>228.99933861109699</v>
+      </c>
+      <c r="O20">
+        <v>153.10575474694599</v>
+      </c>
+      <c r="P20">
+        <v>245.93264469400401</v>
+      </c>
+      <c r="Q20">
+        <v>197.642056920106</v>
+      </c>
+      <c r="R20">
+        <v>107.984927868296</v>
+      </c>
+      <c r="S20" s="3">
         <f t="shared" si="2"/>
-        <v>0</v>
-      </c>
-      <c r="T20" s="2"/>
-      <c r="U20" s="3"/>
-      <c r="V20" s="3"/>
-      <c r="W20" s="3"/>
-      <c r="X20" s="3"/>
-      <c r="Y20" s="3"/>
+        <v>933.66472284044903</v>
+      </c>
+      <c r="T20" s="2">
+        <v>4.7505751848220799</v>
+      </c>
+      <c r="U20">
+        <v>5.2053268432617097</v>
+      </c>
+      <c r="V20">
+        <v>10.8245923757553</v>
+      </c>
+      <c r="W20">
+        <v>7.3275167942047101</v>
+      </c>
+      <c r="X20">
+        <v>1.3861005544662399</v>
+      </c>
+      <c r="Y20" s="3">
+        <f t="shared" si="3"/>
+        <v>29.494111752510037</v>
+      </c>
       <c r="Z20" s="2"/>
       <c r="AA20" s="3"/>
       <c r="AB20" s="3"/>
       <c r="AC20" s="3"/>
       <c r="AD20" s="3"/>
-      <c r="AE20" s="3"/>
+      <c r="AE20" s="5"/>
       <c r="AF20" s="2"/>
       <c r="AG20" s="3"/>
       <c r="AH20" s="3"/>
@@ -2370,17 +2819,16 @@
       <c r="AP20" s="3"/>
       <c r="AQ20" s="3"/>
       <c r="AR20" s="2"/>
-      <c r="AS20" s="3"/>
-      <c r="AT20" s="3"/>
-      <c r="AU20" s="3"/>
-      <c r="AV20" s="3"/>
-      <c r="AW20" s="5"/>
+      <c r="AW20">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="21" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>26</v>
-      </c>
-      <c r="B21">
+        <v>24</v>
+      </c>
+      <c r="B21" s="2">
         <v>396.42721009246401</v>
       </c>
       <c r="C21">
@@ -2418,7 +2866,12 @@
         <f t="shared" si="1"/>
         <v>13.495543456077565</v>
       </c>
-      <c r="S21">
+      <c r="N21" s="2"/>
+      <c r="O21" s="3"/>
+      <c r="P21" s="3"/>
+      <c r="Q21" s="3"/>
+      <c r="R21" s="3"/>
+      <c r="S21" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2427,13 +2880,16 @@
       <c r="V21" s="3"/>
       <c r="W21" s="3"/>
       <c r="X21" s="3"/>
-      <c r="Y21" s="3"/>
+      <c r="Y21" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z21" s="2"/>
       <c r="AA21" s="3"/>
       <c r="AB21" s="3"/>
       <c r="AC21" s="3"/>
       <c r="AD21" s="3"/>
-      <c r="AE21" s="3"/>
+      <c r="AE21" s="5"/>
       <c r="AF21" s="2"/>
       <c r="AG21" s="3"/>
       <c r="AH21" s="3"/>
@@ -2447,17 +2903,16 @@
       <c r="AP21" s="3"/>
       <c r="AQ21" s="3"/>
       <c r="AR21" s="2"/>
-      <c r="AS21" s="3"/>
-      <c r="AT21" s="3"/>
-      <c r="AU21" s="3"/>
-      <c r="AV21" s="3"/>
-      <c r="AW21" s="5"/>
+      <c r="AW21">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>27</v>
-      </c>
-      <c r="B22">
+        <v>25</v>
+      </c>
+      <c r="B22" s="2">
         <v>486.06159273742702</v>
       </c>
       <c r="C22">
@@ -2495,7 +2950,12 @@
         <f t="shared" si="1"/>
         <v>19.044734716415388</v>
       </c>
-      <c r="S22">
+      <c r="N22" s="2"/>
+      <c r="O22" s="3"/>
+      <c r="P22" s="3"/>
+      <c r="Q22" s="3"/>
+      <c r="R22" s="3"/>
+      <c r="S22" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2504,13 +2964,16 @@
       <c r="V22" s="3"/>
       <c r="W22" s="3"/>
       <c r="X22" s="3"/>
-      <c r="Y22" s="3"/>
+      <c r="Y22" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z22" s="2"/>
       <c r="AA22" s="3"/>
       <c r="AB22" s="3"/>
       <c r="AC22" s="3"/>
       <c r="AD22" s="3"/>
-      <c r="AE22" s="3"/>
+      <c r="AE22" s="5"/>
       <c r="AF22" s="2"/>
       <c r="AG22" s="3"/>
       <c r="AH22" s="3"/>
@@ -2524,17 +2987,16 @@
       <c r="AP22" s="3"/>
       <c r="AQ22" s="3"/>
       <c r="AR22" s="2"/>
-      <c r="AS22" s="3"/>
-      <c r="AT22" s="3"/>
-      <c r="AU22" s="3"/>
-      <c r="AV22" s="3"/>
-      <c r="AW22" s="5"/>
+      <c r="AW22">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="23" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>28</v>
-      </c>
-      <c r="B23">
+        <v>26</v>
+      </c>
+      <c r="B23" s="2">
         <v>498.36462739012501</v>
       </c>
       <c r="C23">
@@ -2572,7 +3034,12 @@
         <f t="shared" si="1"/>
         <v>18.263992786407446</v>
       </c>
-      <c r="S23">
+      <c r="N23" s="2"/>
+      <c r="O23" s="3"/>
+      <c r="P23" s="3"/>
+      <c r="Q23" s="3"/>
+      <c r="R23" s="3"/>
+      <c r="S23" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2581,13 +3048,16 @@
       <c r="V23" s="3"/>
       <c r="W23" s="3"/>
       <c r="X23" s="3"/>
-      <c r="Y23" s="3"/>
+      <c r="Y23" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z23" s="2"/>
       <c r="AA23" s="3"/>
       <c r="AB23" s="3"/>
       <c r="AC23" s="3"/>
       <c r="AD23" s="3"/>
-      <c r="AE23" s="3"/>
+      <c r="AE23" s="5"/>
       <c r="AF23" s="2"/>
       <c r="AG23" s="3"/>
       <c r="AH23" s="3"/>
@@ -2601,17 +3071,16 @@
       <c r="AP23" s="3"/>
       <c r="AQ23" s="3"/>
       <c r="AR23" s="2"/>
-      <c r="AS23" s="3"/>
-      <c r="AT23" s="3"/>
-      <c r="AU23" s="3"/>
-      <c r="AV23" s="3"/>
-      <c r="AW23" s="5"/>
+      <c r="AW23">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="24" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>29</v>
-      </c>
-      <c r="B24">
+        <v>27</v>
+      </c>
+      <c r="B24" s="2">
         <v>230.80622383749801</v>
       </c>
       <c r="C24">
@@ -2649,7 +3118,12 @@
         <f t="shared" si="1"/>
         <v>27.142536258697415</v>
       </c>
-      <c r="S24">
+      <c r="N24" s="2"/>
+      <c r="O24" s="3"/>
+      <c r="P24" s="3"/>
+      <c r="Q24" s="3"/>
+      <c r="R24" s="3"/>
+      <c r="S24" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2658,13 +3132,16 @@
       <c r="V24" s="3"/>
       <c r="W24" s="3"/>
       <c r="X24" s="3"/>
-      <c r="Y24" s="3"/>
+      <c r="Y24" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z24" s="2"/>
       <c r="AA24" s="3"/>
       <c r="AB24" s="3"/>
       <c r="AC24" s="3"/>
       <c r="AD24" s="3"/>
-      <c r="AE24" s="3"/>
+      <c r="AE24" s="5"/>
       <c r="AF24" s="2"/>
       <c r="AG24" s="3"/>
       <c r="AH24" s="3"/>
@@ -2678,17 +3155,16 @@
       <c r="AP24" s="3"/>
       <c r="AQ24" s="3"/>
       <c r="AR24" s="2"/>
-      <c r="AS24" s="3"/>
-      <c r="AT24" s="3"/>
-      <c r="AU24" s="3"/>
-      <c r="AV24" s="3"/>
-      <c r="AW24" s="5"/>
+      <c r="AW24">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="25" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>30</v>
-      </c>
-      <c r="B25">
+        <v>28</v>
+      </c>
+      <c r="B25" s="2">
         <v>430.85093028183599</v>
       </c>
       <c r="C25">
@@ -2726,7 +3202,12 @@
         <f t="shared" si="1"/>
         <v>14.727666115760785</v>
       </c>
-      <c r="S25">
+      <c r="N25" s="2"/>
+      <c r="O25" s="3"/>
+      <c r="P25" s="3"/>
+      <c r="Q25" s="3"/>
+      <c r="R25" s="3"/>
+      <c r="S25" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2735,13 +3216,16 @@
       <c r="V25" s="3"/>
       <c r="W25" s="3"/>
       <c r="X25" s="3"/>
-      <c r="Y25" s="3"/>
+      <c r="Y25" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z25" s="2"/>
       <c r="AA25" s="3"/>
       <c r="AB25" s="3"/>
       <c r="AC25" s="3"/>
       <c r="AD25" s="3"/>
-      <c r="AE25" s="3"/>
+      <c r="AE25" s="5"/>
       <c r="AF25" s="2"/>
       <c r="AG25" s="3"/>
       <c r="AH25" s="3"/>
@@ -2755,17 +3239,16 @@
       <c r="AP25" s="3"/>
       <c r="AQ25" s="3"/>
       <c r="AR25" s="2"/>
-      <c r="AS25" s="3"/>
-      <c r="AT25" s="3"/>
-      <c r="AU25" s="3"/>
-      <c r="AV25" s="3"/>
-      <c r="AW25" s="5"/>
+      <c r="AW25">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="26" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>31</v>
-      </c>
-      <c r="B26">
+        <v>29</v>
+      </c>
+      <c r="B26" s="2">
         <v>305.93952909579798</v>
       </c>
       <c r="C26">
@@ -2803,7 +3286,12 @@
         <f t="shared" si="1"/>
         <v>17.819362759590081</v>
       </c>
-      <c r="S26">
+      <c r="N26" s="2"/>
+      <c r="O26" s="3"/>
+      <c r="P26" s="3"/>
+      <c r="Q26" s="3"/>
+      <c r="R26" s="3"/>
+      <c r="S26" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2812,13 +3300,16 @@
       <c r="V26" s="3"/>
       <c r="W26" s="3"/>
       <c r="X26" s="3"/>
-      <c r="Y26" s="3"/>
+      <c r="Y26" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z26" s="2"/>
       <c r="AA26" s="3"/>
       <c r="AB26" s="3"/>
       <c r="AC26" s="3"/>
       <c r="AD26" s="3"/>
-      <c r="AE26" s="3"/>
+      <c r="AE26" s="5"/>
       <c r="AF26" s="2"/>
       <c r="AG26" s="3"/>
       <c r="AH26" s="3"/>
@@ -2832,17 +3323,16 @@
       <c r="AP26" s="3"/>
       <c r="AQ26" s="3"/>
       <c r="AR26" s="2"/>
-      <c r="AS26" s="3"/>
-      <c r="AT26" s="3"/>
-      <c r="AU26" s="3"/>
-      <c r="AV26" s="3"/>
-      <c r="AW26" s="5"/>
+      <c r="AW26">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="27" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>32</v>
-      </c>
-      <c r="B27">
+        <v>30</v>
+      </c>
+      <c r="B27" s="2">
         <v>282.07944490536801</v>
       </c>
       <c r="C27">
@@ -2880,7 +3370,12 @@
         <f t="shared" si="1"/>
         <v>17.645011711120564</v>
       </c>
-      <c r="S27">
+      <c r="N27" s="2"/>
+      <c r="O27" s="3"/>
+      <c r="P27" s="3"/>
+      <c r="Q27" s="3"/>
+      <c r="R27" s="3"/>
+      <c r="S27" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2889,13 +3384,16 @@
       <c r="V27" s="3"/>
       <c r="W27" s="3"/>
       <c r="X27" s="3"/>
-      <c r="Y27" s="3"/>
+      <c r="Y27" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z27" s="2"/>
       <c r="AA27" s="3"/>
       <c r="AB27" s="3"/>
       <c r="AC27" s="3"/>
       <c r="AD27" s="3"/>
-      <c r="AE27" s="3"/>
+      <c r="AE27" s="5"/>
       <c r="AF27" s="2"/>
       <c r="AG27" s="3"/>
       <c r="AH27" s="3"/>
@@ -2909,17 +3407,16 @@
       <c r="AP27" s="3"/>
       <c r="AQ27" s="3"/>
       <c r="AR27" s="2"/>
-      <c r="AS27" s="3"/>
-      <c r="AT27" s="3"/>
-      <c r="AU27" s="3"/>
-      <c r="AV27" s="3"/>
-      <c r="AW27" s="5"/>
+      <c r="AW27">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="28" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>33</v>
-      </c>
-      <c r="B28">
+        <v>31</v>
+      </c>
+      <c r="B28" s="2">
         <v>307.91779029529101</v>
       </c>
       <c r="C28">
@@ -2957,7 +3454,12 @@
         <f t="shared" si="1"/>
         <v>24.068307137489281</v>
       </c>
-      <c r="S28">
+      <c r="N28" s="2"/>
+      <c r="O28" s="3"/>
+      <c r="P28" s="3"/>
+      <c r="Q28" s="3"/>
+      <c r="R28" s="3"/>
+      <c r="S28" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2966,13 +3468,16 @@
       <c r="V28" s="3"/>
       <c r="W28" s="3"/>
       <c r="X28" s="3"/>
-      <c r="Y28" s="3"/>
+      <c r="Y28" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z28" s="2"/>
       <c r="AA28" s="3"/>
       <c r="AB28" s="3"/>
       <c r="AC28" s="3"/>
       <c r="AD28" s="3"/>
-      <c r="AE28" s="3"/>
+      <c r="AE28" s="5"/>
       <c r="AF28" s="2"/>
       <c r="AG28" s="3"/>
       <c r="AH28" s="3"/>
@@ -2986,17 +3491,16 @@
       <c r="AP28" s="3"/>
       <c r="AQ28" s="3"/>
       <c r="AR28" s="2"/>
-      <c r="AS28" s="3"/>
-      <c r="AT28" s="3"/>
-      <c r="AU28" s="3"/>
-      <c r="AV28" s="3"/>
-      <c r="AW28" s="5"/>
+      <c r="AW28">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="29" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>34</v>
-      </c>
-      <c r="B29">
+        <v>32</v>
+      </c>
+      <c r="B29" s="2">
         <v>425.26188515413799</v>
       </c>
       <c r="C29">
@@ -3034,7 +3538,12 @@
         <f t="shared" si="1"/>
         <v>16.758595252037026</v>
       </c>
-      <c r="S29">
+      <c r="N29" s="2"/>
+      <c r="O29" s="3"/>
+      <c r="P29" s="3"/>
+      <c r="Q29" s="3"/>
+      <c r="R29" s="3"/>
+      <c r="S29" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3043,13 +3552,16 @@
       <c r="V29" s="3"/>
       <c r="W29" s="3"/>
       <c r="X29" s="3"/>
-      <c r="Y29" s="3"/>
+      <c r="Y29" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z29" s="2"/>
       <c r="AA29" s="3"/>
       <c r="AB29" s="3"/>
       <c r="AC29" s="3"/>
       <c r="AD29" s="3"/>
-      <c r="AE29" s="3"/>
+      <c r="AE29" s="5"/>
       <c r="AF29" s="2"/>
       <c r="AG29" s="3"/>
       <c r="AH29" s="3"/>
@@ -3063,17 +3575,16 @@
       <c r="AP29" s="3"/>
       <c r="AQ29" s="3"/>
       <c r="AR29" s="2"/>
-      <c r="AS29" s="3"/>
-      <c r="AT29" s="3"/>
-      <c r="AU29" s="3"/>
-      <c r="AV29" s="3"/>
-      <c r="AW29" s="5"/>
+      <c r="AW29">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="30" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>35</v>
-      </c>
-      <c r="B30">
+        <v>33</v>
+      </c>
+      <c r="B30" s="2">
         <v>333.93534490241302</v>
       </c>
       <c r="C30">
@@ -3111,7 +3622,12 @@
         <f t="shared" si="1"/>
         <v>18.732582616806017</v>
       </c>
-      <c r="S30">
+      <c r="N30" s="2"/>
+      <c r="O30" s="3"/>
+      <c r="P30" s="3"/>
+      <c r="Q30" s="3"/>
+      <c r="R30" s="3"/>
+      <c r="S30" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3120,13 +3636,16 @@
       <c r="V30" s="3"/>
       <c r="W30" s="3"/>
       <c r="X30" s="3"/>
-      <c r="Y30" s="3"/>
+      <c r="Y30" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z30" s="2"/>
       <c r="AA30" s="3"/>
       <c r="AB30" s="3"/>
       <c r="AC30" s="3"/>
       <c r="AD30" s="3"/>
-      <c r="AE30" s="3"/>
+      <c r="AE30" s="5"/>
       <c r="AF30" s="2"/>
       <c r="AG30" s="3"/>
       <c r="AH30" s="3"/>
@@ -3140,17 +3659,16 @@
       <c r="AP30" s="3"/>
       <c r="AQ30" s="3"/>
       <c r="AR30" s="2"/>
-      <c r="AS30" s="3"/>
-      <c r="AT30" s="3"/>
-      <c r="AU30" s="3"/>
-      <c r="AV30" s="3"/>
-      <c r="AW30" s="5"/>
+      <c r="AW30">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="31" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>36</v>
-      </c>
-      <c r="B31">
+        <v>34</v>
+      </c>
+      <c r="B31" s="2">
         <v>343.19388904959499</v>
       </c>
       <c r="C31">
@@ -3188,7 +3706,12 @@
         <f t="shared" si="1"/>
         <v>21.763704800605762</v>
       </c>
-      <c r="S31">
+      <c r="N31" s="2"/>
+      <c r="O31" s="3"/>
+      <c r="P31" s="3"/>
+      <c r="Q31" s="3"/>
+      <c r="R31" s="3"/>
+      <c r="S31" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3197,13 +3720,16 @@
       <c r="V31" s="3"/>
       <c r="W31" s="3"/>
       <c r="X31" s="3"/>
-      <c r="Y31" s="3"/>
+      <c r="Y31" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z31" s="2"/>
       <c r="AA31" s="3"/>
       <c r="AB31" s="3"/>
       <c r="AC31" s="3"/>
       <c r="AD31" s="3"/>
-      <c r="AE31" s="3"/>
+      <c r="AE31" s="5"/>
       <c r="AF31" s="2"/>
       <c r="AG31" s="3"/>
       <c r="AH31" s="3"/>
@@ -3217,17 +3743,16 @@
       <c r="AP31" s="3"/>
       <c r="AQ31" s="3"/>
       <c r="AR31" s="2"/>
-      <c r="AS31" s="3"/>
-      <c r="AT31" s="3"/>
-      <c r="AU31" s="3"/>
-      <c r="AV31" s="3"/>
-      <c r="AW31" s="5"/>
+      <c r="AW31">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="32" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>37</v>
-      </c>
-      <c r="B32">
+        <v>35</v>
+      </c>
+      <c r="B32" s="2">
         <v>323.577160567166</v>
       </c>
       <c r="C32">
@@ -3265,7 +3790,12 @@
         <f t="shared" si="1"/>
         <v>25.544930005073478</v>
       </c>
-      <c r="S32">
+      <c r="N32" s="2"/>
+      <c r="O32" s="3"/>
+      <c r="P32" s="3"/>
+      <c r="Q32" s="3"/>
+      <c r="R32" s="3"/>
+      <c r="S32" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3274,13 +3804,16 @@
       <c r="V32" s="3"/>
       <c r="W32" s="3"/>
       <c r="X32" s="3"/>
-      <c r="Y32" s="3"/>
+      <c r="Y32" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z32" s="2"/>
       <c r="AA32" s="3"/>
       <c r="AB32" s="3"/>
       <c r="AC32" s="3"/>
       <c r="AD32" s="3"/>
-      <c r="AE32" s="3"/>
+      <c r="AE32" s="5"/>
       <c r="AF32" s="2"/>
       <c r="AG32" s="3"/>
       <c r="AH32" s="3"/>
@@ -3294,35 +3827,59 @@
       <c r="AP32" s="3"/>
       <c r="AQ32" s="3"/>
       <c r="AR32" s="2"/>
-      <c r="AS32" s="3"/>
-      <c r="AT32" s="3"/>
-      <c r="AU32" s="3"/>
-      <c r="AV32" s="3"/>
-      <c r="AW32" s="5"/>
+      <c r="AW32">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="33" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>38</v>
-      </c>
-      <c r="B33" s="2"/>
-      <c r="C33" s="3"/>
-      <c r="D33" s="3"/>
-      <c r="E33" s="3"/>
-      <c r="F33" s="3"/>
+        <v>36</v>
+      </c>
+      <c r="B33" s="2">
+        <v>388.94166662511202</v>
+      </c>
+      <c r="C33">
+        <v>289.31228206488902</v>
+      </c>
+      <c r="D33">
+        <v>82.919690152818902</v>
+      </c>
+      <c r="E33">
+        <v>498.84729163273198</v>
+      </c>
+      <c r="F33">
+        <v>163.572197532601</v>
+      </c>
       <c r="G33" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H33" s="2"/>
-      <c r="I33" s="3"/>
-      <c r="J33" s="3"/>
-      <c r="K33" s="3"/>
-      <c r="L33" s="3"/>
+        <v>1423.5931280081529</v>
+      </c>
+      <c r="H33">
+        <v>5.1738923788070599</v>
+      </c>
+      <c r="I33">
+        <v>1.90940163135528</v>
+      </c>
+      <c r="J33">
+        <v>0.422524762153625</v>
+      </c>
+      <c r="K33">
+        <v>14.501803088188099</v>
+      </c>
+      <c r="L33">
+        <v>1.08075559139251</v>
+      </c>
       <c r="M33" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S33">
+        <v>23.088377451896573</v>
+      </c>
+      <c r="N33" s="2"/>
+      <c r="O33" s="3"/>
+      <c r="P33" s="3"/>
+      <c r="Q33" s="3"/>
+      <c r="R33" s="3"/>
+      <c r="S33" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3331,13 +3888,16 @@
       <c r="V33" s="3"/>
       <c r="W33" s="3"/>
       <c r="X33" s="3"/>
-      <c r="Y33" s="3"/>
+      <c r="Y33" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z33" s="2"/>
       <c r="AA33" s="3"/>
       <c r="AB33" s="3"/>
       <c r="AC33" s="3"/>
       <c r="AD33" s="3"/>
-      <c r="AE33" s="3"/>
+      <c r="AE33" s="5"/>
       <c r="AF33" s="2"/>
       <c r="AG33" s="3"/>
       <c r="AH33" s="3"/>
@@ -3351,35 +3911,59 @@
       <c r="AP33" s="3"/>
       <c r="AQ33" s="3"/>
       <c r="AR33" s="2"/>
-      <c r="AS33" s="3"/>
-      <c r="AT33" s="3"/>
-      <c r="AU33" s="3"/>
-      <c r="AV33" s="3"/>
-      <c r="AW33" s="5"/>
+      <c r="AW33">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="34" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>39</v>
-      </c>
-      <c r="B34" s="2"/>
-      <c r="C34" s="3"/>
-      <c r="D34" s="3"/>
-      <c r="E34" s="3"/>
-      <c r="F34" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="B34" s="2">
+        <v>424.91878847256402</v>
+      </c>
+      <c r="C34">
+        <v>387.99785407911099</v>
+      </c>
+      <c r="D34">
+        <v>86.2919458469094</v>
+      </c>
+      <c r="E34">
+        <v>515.19837385572703</v>
+      </c>
+      <c r="F34">
+        <v>125.12396970734601</v>
+      </c>
       <c r="G34" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H34" s="2"/>
-      <c r="I34" s="3"/>
-      <c r="J34" s="3"/>
-      <c r="K34" s="3"/>
-      <c r="L34" s="3"/>
+        <v>1539.5309319616576</v>
+      </c>
+      <c r="H34">
+        <v>11.0200849056243</v>
+      </c>
+      <c r="I34">
+        <v>3.9728592395782401</v>
+      </c>
+      <c r="J34">
+        <v>0.309067106246948</v>
+      </c>
+      <c r="K34">
+        <v>60.8533322811126</v>
+      </c>
+      <c r="L34">
+        <v>0.413281345367431</v>
+      </c>
       <c r="M34" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S34">
+        <v>76.568624877929523</v>
+      </c>
+      <c r="N34" s="2"/>
+      <c r="O34" s="3"/>
+      <c r="P34" s="3"/>
+      <c r="Q34" s="3"/>
+      <c r="R34" s="3"/>
+      <c r="S34" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3388,13 +3972,16 @@
       <c r="V34" s="3"/>
       <c r="W34" s="3"/>
       <c r="X34" s="3"/>
-      <c r="Y34" s="3"/>
+      <c r="Y34" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z34" s="2"/>
       <c r="AA34" s="3"/>
       <c r="AB34" s="3"/>
       <c r="AC34" s="3"/>
       <c r="AD34" s="3"/>
-      <c r="AE34" s="3"/>
+      <c r="AE34" s="5"/>
       <c r="AF34" s="2"/>
       <c r="AG34" s="3"/>
       <c r="AH34" s="3"/>
@@ -3408,35 +3995,59 @@
       <c r="AP34" s="3"/>
       <c r="AQ34" s="3"/>
       <c r="AR34" s="2"/>
-      <c r="AS34" s="3"/>
-      <c r="AT34" s="3"/>
-      <c r="AU34" s="3"/>
-      <c r="AV34" s="3"/>
-      <c r="AW34" s="5"/>
+      <c r="AW34">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="35" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>40</v>
-      </c>
-      <c r="B35" s="2"/>
-      <c r="C35" s="3"/>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
-      <c r="F35" s="3"/>
+        <v>38</v>
+      </c>
+      <c r="B35" s="2">
+        <v>449.41272167038699</v>
+      </c>
+      <c r="C35">
+        <v>226.021249866885</v>
+      </c>
+      <c r="D35">
+        <v>67.633291343977703</v>
+      </c>
+      <c r="E35">
+        <v>561.74339957116695</v>
+      </c>
+      <c r="F35">
+        <v>99.011563715914207</v>
+      </c>
       <c r="G35" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H35" s="2"/>
-      <c r="I35" s="3"/>
-      <c r="J35" s="3"/>
-      <c r="K35" s="3"/>
-      <c r="L35" s="3"/>
+        <v>1403.8222261683309</v>
+      </c>
+      <c r="H35">
+        <v>18.133386349677998</v>
+      </c>
+      <c r="I35">
+        <v>2.2179700136184599</v>
+      </c>
+      <c r="J35">
+        <v>0.43875973224639803</v>
+      </c>
+      <c r="K35">
+        <v>62.954458427429202</v>
+      </c>
+      <c r="L35">
+        <v>0.65681362152099598</v>
+      </c>
       <c r="M35" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S35">
+        <v>84.401388144493055</v>
+      </c>
+      <c r="N35" s="2"/>
+      <c r="O35" s="3"/>
+      <c r="P35" s="3"/>
+      <c r="Q35" s="3"/>
+      <c r="R35" s="3"/>
+      <c r="S35" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3445,13 +4056,16 @@
       <c r="V35" s="3"/>
       <c r="W35" s="3"/>
       <c r="X35" s="3"/>
-      <c r="Y35" s="3"/>
+      <c r="Y35" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z35" s="2"/>
       <c r="AA35" s="3"/>
       <c r="AB35" s="3"/>
       <c r="AC35" s="3"/>
       <c r="AD35" s="3"/>
-      <c r="AE35" s="3"/>
+      <c r="AE35" s="5"/>
       <c r="AF35" s="2"/>
       <c r="AG35" s="3"/>
       <c r="AH35" s="3"/>
@@ -3465,35 +4079,59 @@
       <c r="AP35" s="3"/>
       <c r="AQ35" s="3"/>
       <c r="AR35" s="2"/>
-      <c r="AS35" s="3"/>
-      <c r="AT35" s="3"/>
-      <c r="AU35" s="3"/>
-      <c r="AV35" s="3"/>
-      <c r="AW35" s="5"/>
+      <c r="AW35">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="36" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>41</v>
-      </c>
-      <c r="B36" s="2"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
-      <c r="F36" s="3"/>
+        <v>39</v>
+      </c>
+      <c r="B36" s="2">
+        <v>597.53672294878095</v>
+      </c>
+      <c r="C36">
+        <v>142.180987029607</v>
+      </c>
+      <c r="D36">
+        <v>54.823998668695097</v>
+      </c>
+      <c r="E36">
+        <v>400.04271665790702</v>
+      </c>
+      <c r="F36">
+        <v>107.08189412704</v>
+      </c>
       <c r="G36" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H36" s="2"/>
-      <c r="I36" s="3"/>
-      <c r="J36" s="3"/>
-      <c r="K36" s="3"/>
-      <c r="L36" s="3"/>
+        <v>1301.6663194320299</v>
+      </c>
+      <c r="H36">
+        <v>167.62043120861</v>
+      </c>
+      <c r="I36">
+        <v>0.72630040645599303</v>
+      </c>
+      <c r="J36">
+        <v>0.31340832710266098</v>
+      </c>
+      <c r="K36">
+        <v>88.399788379669104</v>
+      </c>
+      <c r="L36">
+        <v>0.44311192035675001</v>
+      </c>
       <c r="M36" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S36">
+        <v>257.50304024219452</v>
+      </c>
+      <c r="N36" s="2"/>
+      <c r="O36" s="3"/>
+      <c r="P36" s="3"/>
+      <c r="Q36" s="3"/>
+      <c r="R36" s="3"/>
+      <c r="S36" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3502,13 +4140,16 @@
       <c r="V36" s="3"/>
       <c r="W36" s="3"/>
       <c r="X36" s="3"/>
-      <c r="Y36" s="3"/>
+      <c r="Y36" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z36" s="2"/>
       <c r="AA36" s="3"/>
       <c r="AB36" s="3"/>
       <c r="AC36" s="3"/>
       <c r="AD36" s="3"/>
-      <c r="AE36" s="3"/>
+      <c r="AE36" s="5"/>
       <c r="AF36" s="2"/>
       <c r="AG36" s="3"/>
       <c r="AH36" s="3"/>
@@ -3522,15 +4163,14 @@
       <c r="AP36" s="3"/>
       <c r="AQ36" s="3"/>
       <c r="AR36" s="2"/>
-      <c r="AS36" s="3"/>
-      <c r="AT36" s="3"/>
-      <c r="AU36" s="3"/>
-      <c r="AV36" s="3"/>
-      <c r="AW36" s="5"/>
+      <c r="AW36">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="37" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="3"/>
@@ -3550,7 +4190,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S37">
+      <c r="N37" s="2"/>
+      <c r="O37" s="3"/>
+      <c r="P37" s="3"/>
+      <c r="Q37" s="3"/>
+      <c r="R37" s="3"/>
+      <c r="S37" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3559,13 +4204,16 @@
       <c r="V37" s="3"/>
       <c r="W37" s="3"/>
       <c r="X37" s="3"/>
-      <c r="Y37" s="3"/>
+      <c r="Y37" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z37" s="2"/>
       <c r="AA37" s="3"/>
       <c r="AB37" s="3"/>
       <c r="AC37" s="3"/>
       <c r="AD37" s="3"/>
-      <c r="AE37" s="3"/>
+      <c r="AE37" s="5"/>
       <c r="AF37" s="2"/>
       <c r="AG37" s="3"/>
       <c r="AH37" s="3"/>
@@ -3579,15 +4227,14 @@
       <c r="AP37" s="3"/>
       <c r="AQ37" s="3"/>
       <c r="AR37" s="2"/>
-      <c r="AS37" s="3"/>
-      <c r="AT37" s="3"/>
-      <c r="AU37" s="3"/>
-      <c r="AV37" s="3"/>
-      <c r="AW37" s="5"/>
+      <c r="AW37">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="38" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B38" s="2"/>
       <c r="C38" s="3"/>
@@ -3607,7 +4254,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S38">
+      <c r="N38" s="2"/>
+      <c r="O38" s="3"/>
+      <c r="P38" s="3"/>
+      <c r="Q38" s="3"/>
+      <c r="R38" s="3"/>
+      <c r="S38" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3616,13 +4268,16 @@
       <c r="V38" s="3"/>
       <c r="W38" s="3"/>
       <c r="X38" s="3"/>
-      <c r="Y38" s="3"/>
+      <c r="Y38" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z38" s="2"/>
       <c r="AA38" s="3"/>
       <c r="AB38" s="3"/>
       <c r="AC38" s="3"/>
       <c r="AD38" s="3"/>
-      <c r="AE38" s="3"/>
+      <c r="AE38" s="5"/>
       <c r="AF38" s="2"/>
       <c r="AG38" s="3"/>
       <c r="AH38" s="3"/>
@@ -3636,15 +4291,14 @@
       <c r="AP38" s="3"/>
       <c r="AQ38" s="3"/>
       <c r="AR38" s="2"/>
-      <c r="AS38" s="3"/>
-      <c r="AT38" s="3"/>
-      <c r="AU38" s="3"/>
-      <c r="AV38" s="3"/>
-      <c r="AW38" s="5"/>
+      <c r="AW38">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="39" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B39" s="2"/>
       <c r="C39" s="3"/>
@@ -3664,7 +4318,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S39">
+      <c r="N39" s="2"/>
+      <c r="O39" s="3"/>
+      <c r="P39" s="3"/>
+      <c r="Q39" s="3"/>
+      <c r="R39" s="3"/>
+      <c r="S39" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3673,13 +4332,16 @@
       <c r="V39" s="3"/>
       <c r="W39" s="3"/>
       <c r="X39" s="3"/>
-      <c r="Y39" s="3"/>
+      <c r="Y39" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z39" s="2"/>
       <c r="AA39" s="3"/>
       <c r="AB39" s="3"/>
       <c r="AC39" s="3"/>
       <c r="AD39" s="3"/>
-      <c r="AE39" s="3"/>
+      <c r="AE39" s="5"/>
       <c r="AF39" s="2"/>
       <c r="AG39" s="3"/>
       <c r="AH39" s="3"/>
@@ -3693,15 +4355,14 @@
       <c r="AP39" s="3"/>
       <c r="AQ39" s="3"/>
       <c r="AR39" s="2"/>
-      <c r="AS39" s="3"/>
-      <c r="AT39" s="3"/>
-      <c r="AU39" s="3"/>
-      <c r="AV39" s="3"/>
-      <c r="AW39" s="5"/>
+      <c r="AW39">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="40" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B40" s="2"/>
       <c r="C40" s="3"/>
@@ -3721,7 +4382,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S40">
+      <c r="N40" s="2"/>
+      <c r="O40" s="3"/>
+      <c r="P40" s="3"/>
+      <c r="Q40" s="3"/>
+      <c r="R40" s="3"/>
+      <c r="S40" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3730,13 +4396,16 @@
       <c r="V40" s="3"/>
       <c r="W40" s="3"/>
       <c r="X40" s="3"/>
-      <c r="Y40" s="3"/>
+      <c r="Y40" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z40" s="2"/>
       <c r="AA40" s="3"/>
       <c r="AB40" s="3"/>
       <c r="AC40" s="3"/>
       <c r="AD40" s="3"/>
-      <c r="AE40" s="3"/>
+      <c r="AE40" s="5"/>
       <c r="AF40" s="2"/>
       <c r="AG40" s="3"/>
       <c r="AH40" s="3"/>
@@ -3750,15 +4419,14 @@
       <c r="AP40" s="3"/>
       <c r="AQ40" s="3"/>
       <c r="AR40" s="2"/>
-      <c r="AS40" s="3"/>
-      <c r="AT40" s="3"/>
-      <c r="AU40" s="3"/>
-      <c r="AV40" s="3"/>
-      <c r="AW40" s="5"/>
+      <c r="AW40">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="41" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B41" s="2"/>
       <c r="C41" s="3"/>
@@ -3778,7 +4446,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S41">
+      <c r="N41" s="2"/>
+      <c r="O41" s="3"/>
+      <c r="P41" s="3"/>
+      <c r="Q41" s="3"/>
+      <c r="R41" s="3"/>
+      <c r="S41" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3787,13 +4460,16 @@
       <c r="V41" s="3"/>
       <c r="W41" s="3"/>
       <c r="X41" s="3"/>
-      <c r="Y41" s="3"/>
+      <c r="Y41" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z41" s="2"/>
       <c r="AA41" s="3"/>
       <c r="AB41" s="3"/>
       <c r="AC41" s="3"/>
       <c r="AD41" s="3"/>
-      <c r="AE41" s="3"/>
+      <c r="AE41" s="5"/>
       <c r="AF41" s="2"/>
       <c r="AG41" s="3"/>
       <c r="AH41" s="3"/>
@@ -3807,15 +4483,14 @@
       <c r="AP41" s="3"/>
       <c r="AQ41" s="3"/>
       <c r="AR41" s="2"/>
-      <c r="AS41" s="3"/>
-      <c r="AT41" s="3"/>
-      <c r="AU41" s="3"/>
-      <c r="AV41" s="3"/>
-      <c r="AW41" s="5"/>
+      <c r="AW41">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="42" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B42" s="2"/>
       <c r="C42" s="3"/>
@@ -3835,7 +4510,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S42">
+      <c r="N42" s="2"/>
+      <c r="O42" s="3"/>
+      <c r="P42" s="3"/>
+      <c r="Q42" s="3"/>
+      <c r="R42" s="3"/>
+      <c r="S42" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3844,13 +4524,16 @@
       <c r="V42" s="3"/>
       <c r="W42" s="3"/>
       <c r="X42" s="3"/>
-      <c r="Y42" s="3"/>
+      <c r="Y42" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z42" s="2"/>
       <c r="AA42" s="3"/>
       <c r="AB42" s="3"/>
       <c r="AC42" s="3"/>
       <c r="AD42" s="3"/>
-      <c r="AE42" s="3"/>
+      <c r="AE42" s="5"/>
       <c r="AF42" s="2"/>
       <c r="AG42" s="3"/>
       <c r="AH42" s="3"/>
@@ -3864,15 +4547,14 @@
       <c r="AP42" s="3"/>
       <c r="AQ42" s="3"/>
       <c r="AR42" s="2"/>
-      <c r="AS42" s="3"/>
-      <c r="AT42" s="3"/>
-      <c r="AU42" s="3"/>
-      <c r="AV42" s="3"/>
-      <c r="AW42" s="5"/>
+      <c r="AW42">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="43" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B43" s="2"/>
       <c r="C43" s="3"/>
@@ -3892,7 +4574,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S43">
+      <c r="N43" s="2"/>
+      <c r="O43" s="3"/>
+      <c r="P43" s="3"/>
+      <c r="Q43" s="3"/>
+      <c r="R43" s="3"/>
+      <c r="S43" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3901,13 +4588,16 @@
       <c r="V43" s="3"/>
       <c r="W43" s="3"/>
       <c r="X43" s="3"/>
-      <c r="Y43" s="3"/>
+      <c r="Y43" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z43" s="2"/>
       <c r="AA43" s="3"/>
       <c r="AB43" s="3"/>
       <c r="AC43" s="3"/>
       <c r="AD43" s="3"/>
-      <c r="AE43" s="3"/>
+      <c r="AE43" s="5"/>
       <c r="AF43" s="2"/>
       <c r="AG43" s="3"/>
       <c r="AH43" s="3"/>
@@ -3921,15 +4611,14 @@
       <c r="AP43" s="3"/>
       <c r="AQ43" s="3"/>
       <c r="AR43" s="2"/>
-      <c r="AS43" s="3"/>
-      <c r="AT43" s="3"/>
-      <c r="AU43" s="3"/>
-      <c r="AV43" s="3"/>
-      <c r="AW43" s="5"/>
+      <c r="AW43">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="44" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="B44" s="2"/>
       <c r="C44" s="3"/>
@@ -3949,7 +4638,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S44">
+      <c r="N44" s="2"/>
+      <c r="O44" s="3"/>
+      <c r="P44" s="3"/>
+      <c r="Q44" s="3"/>
+      <c r="R44" s="3"/>
+      <c r="S44" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -3958,13 +4652,16 @@
       <c r="V44" s="3"/>
       <c r="W44" s="3"/>
       <c r="X44" s="3"/>
-      <c r="Y44" s="3"/>
+      <c r="Y44" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z44" s="2"/>
       <c r="AA44" s="3"/>
       <c r="AB44" s="3"/>
       <c r="AC44" s="3"/>
       <c r="AD44" s="3"/>
-      <c r="AE44" s="3"/>
+      <c r="AE44" s="5"/>
       <c r="AF44" s="2"/>
       <c r="AG44" s="3"/>
       <c r="AH44" s="3"/>
@@ -3978,15 +4675,14 @@
       <c r="AP44" s="3"/>
       <c r="AQ44" s="3"/>
       <c r="AR44" s="2"/>
-      <c r="AS44" s="3"/>
-      <c r="AT44" s="3"/>
-      <c r="AU44" s="3"/>
-      <c r="AV44" s="3"/>
-      <c r="AW44" s="5"/>
+      <c r="AW44">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="45" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B45" s="2"/>
       <c r="C45" s="3"/>
@@ -4006,7 +4702,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S45">
+      <c r="N45" s="2"/>
+      <c r="O45" s="3"/>
+      <c r="P45" s="3"/>
+      <c r="Q45" s="3"/>
+      <c r="R45" s="3"/>
+      <c r="S45" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4015,13 +4716,16 @@
       <c r="V45" s="3"/>
       <c r="W45" s="3"/>
       <c r="X45" s="3"/>
-      <c r="Y45" s="3"/>
+      <c r="Y45" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z45" s="2"/>
       <c r="AA45" s="3"/>
       <c r="AB45" s="3"/>
       <c r="AC45" s="3"/>
       <c r="AD45" s="3"/>
-      <c r="AE45" s="3"/>
+      <c r="AE45" s="5"/>
       <c r="AF45" s="2"/>
       <c r="AG45" s="3"/>
       <c r="AH45" s="3"/>
@@ -4035,15 +4739,14 @@
       <c r="AP45" s="3"/>
       <c r="AQ45" s="3"/>
       <c r="AR45" s="2"/>
-      <c r="AS45" s="3"/>
-      <c r="AT45" s="3"/>
-      <c r="AU45" s="3"/>
-      <c r="AV45" s="3"/>
-      <c r="AW45" s="5"/>
+      <c r="AW45">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="46" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B46" s="2"/>
       <c r="C46" s="3"/>
@@ -4063,7 +4766,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S46">
+      <c r="N46" s="2"/>
+      <c r="O46" s="3"/>
+      <c r="P46" s="3"/>
+      <c r="Q46" s="3"/>
+      <c r="R46" s="3"/>
+      <c r="S46" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4072,13 +4780,16 @@
       <c r="V46" s="3"/>
       <c r="W46" s="3"/>
       <c r="X46" s="3"/>
-      <c r="Y46" s="3"/>
+      <c r="Y46" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z46" s="2"/>
       <c r="AA46" s="3"/>
       <c r="AB46" s="3"/>
       <c r="AC46" s="3"/>
       <c r="AD46" s="3"/>
-      <c r="AE46" s="3"/>
+      <c r="AE46" s="5"/>
       <c r="AF46" s="2"/>
       <c r="AG46" s="3"/>
       <c r="AH46" s="3"/>
@@ -4092,15 +4803,14 @@
       <c r="AP46" s="3"/>
       <c r="AQ46" s="3"/>
       <c r="AR46" s="2"/>
-      <c r="AS46" s="3"/>
-      <c r="AT46" s="3"/>
-      <c r="AU46" s="3"/>
-      <c r="AV46" s="3"/>
-      <c r="AW46" s="5"/>
+      <c r="AW46">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="47" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B47" s="2"/>
       <c r="C47" s="3"/>
@@ -4120,7 +4830,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S47">
+      <c r="N47" s="2"/>
+      <c r="O47" s="3"/>
+      <c r="P47" s="3"/>
+      <c r="Q47" s="3"/>
+      <c r="R47" s="3"/>
+      <c r="S47" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4129,13 +4844,16 @@
       <c r="V47" s="3"/>
       <c r="W47" s="3"/>
       <c r="X47" s="3"/>
-      <c r="Y47" s="3"/>
+      <c r="Y47" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z47" s="2"/>
       <c r="AA47" s="3"/>
       <c r="AB47" s="3"/>
       <c r="AC47" s="3"/>
       <c r="AD47" s="3"/>
-      <c r="AE47" s="3"/>
+      <c r="AE47" s="5"/>
       <c r="AF47" s="2"/>
       <c r="AG47" s="3"/>
       <c r="AH47" s="3"/>
@@ -4149,15 +4867,14 @@
       <c r="AP47" s="3"/>
       <c r="AQ47" s="3"/>
       <c r="AR47" s="2"/>
-      <c r="AS47" s="3"/>
-      <c r="AT47" s="3"/>
-      <c r="AU47" s="3"/>
-      <c r="AV47" s="3"/>
-      <c r="AW47" s="5"/>
+      <c r="AW47">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="48" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B48" s="2"/>
       <c r="C48" s="3"/>
@@ -4177,7 +4894,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S48">
+      <c r="N48" s="2"/>
+      <c r="O48" s="3"/>
+      <c r="P48" s="3"/>
+      <c r="Q48" s="3"/>
+      <c r="R48" s="3"/>
+      <c r="S48" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4186,13 +4908,16 @@
       <c r="V48" s="3"/>
       <c r="W48" s="3"/>
       <c r="X48" s="3"/>
-      <c r="Y48" s="3"/>
+      <c r="Y48" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z48" s="2"/>
       <c r="AA48" s="3"/>
       <c r="AB48" s="3"/>
       <c r="AC48" s="3"/>
       <c r="AD48" s="3"/>
-      <c r="AE48" s="3"/>
+      <c r="AE48" s="5"/>
       <c r="AF48" s="2"/>
       <c r="AG48" s="3"/>
       <c r="AH48" s="3"/>
@@ -4206,15 +4931,14 @@
       <c r="AP48" s="3"/>
       <c r="AQ48" s="3"/>
       <c r="AR48" s="2"/>
-      <c r="AS48" s="3"/>
-      <c r="AT48" s="3"/>
-      <c r="AU48" s="3"/>
-      <c r="AV48" s="3"/>
-      <c r="AW48" s="5"/>
+      <c r="AW48">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="49" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="3"/>
@@ -4234,7 +4958,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S49">
+      <c r="N49" s="2"/>
+      <c r="O49" s="3"/>
+      <c r="P49" s="3"/>
+      <c r="Q49" s="3"/>
+      <c r="R49" s="3"/>
+      <c r="S49" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4243,13 +4972,16 @@
       <c r="V49" s="3"/>
       <c r="W49" s="3"/>
       <c r="X49" s="3"/>
-      <c r="Y49" s="3"/>
+      <c r="Y49" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z49" s="2"/>
       <c r="AA49" s="3"/>
       <c r="AB49" s="3"/>
       <c r="AC49" s="3"/>
       <c r="AD49" s="3"/>
-      <c r="AE49" s="3"/>
+      <c r="AE49" s="5"/>
       <c r="AF49" s="2"/>
       <c r="AG49" s="3"/>
       <c r="AH49" s="3"/>
@@ -4263,15 +4995,14 @@
       <c r="AP49" s="3"/>
       <c r="AQ49" s="3"/>
       <c r="AR49" s="2"/>
-      <c r="AS49" s="3"/>
-      <c r="AT49" s="3"/>
-      <c r="AU49" s="3"/>
-      <c r="AV49" s="3"/>
-      <c r="AW49" s="5"/>
+      <c r="AW49">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="50" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B50" s="2"/>
       <c r="C50" s="3"/>
@@ -4291,7 +5022,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S50">
+      <c r="N50" s="2"/>
+      <c r="O50" s="3"/>
+      <c r="P50" s="3"/>
+      <c r="Q50" s="3"/>
+      <c r="R50" s="3"/>
+      <c r="S50" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4300,13 +5036,16 @@
       <c r="V50" s="3"/>
       <c r="W50" s="3"/>
       <c r="X50" s="3"/>
-      <c r="Y50" s="3"/>
+      <c r="Y50" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z50" s="2"/>
       <c r="AA50" s="3"/>
       <c r="AB50" s="3"/>
       <c r="AC50" s="3"/>
       <c r="AD50" s="3"/>
-      <c r="AE50" s="3"/>
+      <c r="AE50" s="5"/>
       <c r="AF50" s="2"/>
       <c r="AG50" s="3"/>
       <c r="AH50" s="3"/>
@@ -4320,15 +5059,14 @@
       <c r="AP50" s="3"/>
       <c r="AQ50" s="3"/>
       <c r="AR50" s="2"/>
-      <c r="AS50" s="3"/>
-      <c r="AT50" s="3"/>
-      <c r="AU50" s="3"/>
-      <c r="AV50" s="3"/>
-      <c r="AW50" s="5"/>
+      <c r="AW50">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="51" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="B51" s="2"/>
       <c r="C51" s="3"/>
@@ -4348,7 +5086,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S51">
+      <c r="N51" s="2"/>
+      <c r="O51" s="3"/>
+      <c r="P51" s="3"/>
+      <c r="Q51" s="3"/>
+      <c r="R51" s="3"/>
+      <c r="S51" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4357,13 +5100,16 @@
       <c r="V51" s="3"/>
       <c r="W51" s="3"/>
       <c r="X51" s="3"/>
-      <c r="Y51" s="3"/>
+      <c r="Y51" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z51" s="2"/>
       <c r="AA51" s="3"/>
       <c r="AB51" s="3"/>
       <c r="AC51" s="3"/>
       <c r="AD51" s="3"/>
-      <c r="AE51" s="3"/>
+      <c r="AE51" s="5"/>
       <c r="AF51" s="2"/>
       <c r="AG51" s="3"/>
       <c r="AH51" s="3"/>
@@ -4377,15 +5123,14 @@
       <c r="AP51" s="3"/>
       <c r="AQ51" s="3"/>
       <c r="AR51" s="2"/>
-      <c r="AS51" s="3"/>
-      <c r="AT51" s="3"/>
-      <c r="AU51" s="3"/>
-      <c r="AV51" s="3"/>
-      <c r="AW51" s="5"/>
+      <c r="AW51">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="52" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B52" s="2"/>
       <c r="C52" s="3"/>
@@ -4405,7 +5150,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S52">
+      <c r="N52" s="2"/>
+      <c r="O52" s="3"/>
+      <c r="P52" s="3"/>
+      <c r="Q52" s="3"/>
+      <c r="R52" s="3"/>
+      <c r="S52" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4414,13 +5164,16 @@
       <c r="V52" s="3"/>
       <c r="W52" s="3"/>
       <c r="X52" s="3"/>
-      <c r="Y52" s="3"/>
+      <c r="Y52" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z52" s="2"/>
       <c r="AA52" s="3"/>
       <c r="AB52" s="3"/>
       <c r="AC52" s="3"/>
       <c r="AD52" s="3"/>
-      <c r="AE52" s="3"/>
+      <c r="AE52" s="5"/>
       <c r="AF52" s="2"/>
       <c r="AG52" s="3"/>
       <c r="AH52" s="3"/>
@@ -4434,15 +5187,14 @@
       <c r="AP52" s="3"/>
       <c r="AQ52" s="3"/>
       <c r="AR52" s="2"/>
-      <c r="AS52" s="3"/>
-      <c r="AT52" s="3"/>
-      <c r="AU52" s="3"/>
-      <c r="AV52" s="3"/>
-      <c r="AW52" s="5"/>
+      <c r="AW52">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="53" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B53" s="2"/>
       <c r="C53" s="3"/>
@@ -4462,7 +5214,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S53">
+      <c r="N53" s="2"/>
+      <c r="O53" s="3"/>
+      <c r="P53" s="3"/>
+      <c r="Q53" s="3"/>
+      <c r="R53" s="3"/>
+      <c r="S53" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4471,13 +5228,16 @@
       <c r="V53" s="3"/>
       <c r="W53" s="3"/>
       <c r="X53" s="3"/>
-      <c r="Y53" s="3"/>
+      <c r="Y53" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z53" s="2"/>
       <c r="AA53" s="3"/>
       <c r="AB53" s="3"/>
       <c r="AC53" s="3"/>
       <c r="AD53" s="3"/>
-      <c r="AE53" s="3"/>
+      <c r="AE53" s="5"/>
       <c r="AF53" s="2"/>
       <c r="AG53" s="3"/>
       <c r="AH53" s="3"/>
@@ -4491,15 +5251,14 @@
       <c r="AP53" s="3"/>
       <c r="AQ53" s="3"/>
       <c r="AR53" s="2"/>
-      <c r="AS53" s="3"/>
-      <c r="AT53" s="3"/>
-      <c r="AU53" s="3"/>
-      <c r="AV53" s="3"/>
-      <c r="AW53" s="5"/>
+      <c r="AW53">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="54" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B54" s="2"/>
       <c r="C54" s="3"/>
@@ -4519,7 +5278,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S54">
+      <c r="N54" s="2"/>
+      <c r="O54" s="3"/>
+      <c r="P54" s="3"/>
+      <c r="Q54" s="3"/>
+      <c r="R54" s="3"/>
+      <c r="S54" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4528,13 +5292,16 @@
       <c r="V54" s="3"/>
       <c r="W54" s="3"/>
       <c r="X54" s="3"/>
-      <c r="Y54" s="3"/>
+      <c r="Y54" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z54" s="2"/>
       <c r="AA54" s="3"/>
       <c r="AB54" s="3"/>
       <c r="AC54" s="3"/>
       <c r="AD54" s="3"/>
-      <c r="AE54" s="3"/>
+      <c r="AE54" s="5"/>
       <c r="AF54" s="2"/>
       <c r="AG54" s="3"/>
       <c r="AH54" s="3"/>
@@ -4548,35 +5315,59 @@
       <c r="AP54" s="3"/>
       <c r="AQ54" s="3"/>
       <c r="AR54" s="2"/>
-      <c r="AS54" s="3"/>
-      <c r="AT54" s="3"/>
-      <c r="AU54" s="3"/>
-      <c r="AV54" s="3"/>
-      <c r="AW54" s="5"/>
+      <c r="AW54">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="55" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>60</v>
-      </c>
-      <c r="B55" s="2"/>
-      <c r="C55" s="3"/>
-      <c r="D55" s="3"/>
-      <c r="E55" s="3"/>
-      <c r="F55" s="3"/>
+        <v>58</v>
+      </c>
+      <c r="B55" s="2">
+        <v>176.857853206957</v>
+      </c>
+      <c r="C55">
+        <v>229.655401893224</v>
+      </c>
+      <c r="D55">
+        <v>87.002554733232202</v>
+      </c>
+      <c r="E55">
+        <v>359.06462829200899</v>
+      </c>
+      <c r="F55">
+        <v>300.77546920872902</v>
+      </c>
       <c r="G55" s="5">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H55" s="2"/>
-      <c r="I55" s="3"/>
-      <c r="J55" s="3"/>
-      <c r="K55" s="3"/>
-      <c r="L55" s="3"/>
+        <v>1153.3559073341512</v>
+      </c>
+      <c r="H55">
+        <v>1.7515081644058199</v>
+      </c>
+      <c r="I55">
+        <v>15.043546414375299</v>
+      </c>
+      <c r="J55">
+        <v>1.6562985181808401</v>
+      </c>
+      <c r="K55">
+        <v>54.908089995384202</v>
+      </c>
+      <c r="L55">
+        <v>27.5960756540298</v>
+      </c>
       <c r="M55" s="5">
         <f t="shared" si="1"/>
-        <v>0</v>
-      </c>
-      <c r="S55">
+        <v>100.95551874637597</v>
+      </c>
+      <c r="N55" s="2"/>
+      <c r="O55" s="3"/>
+      <c r="P55" s="3"/>
+      <c r="Q55" s="3"/>
+      <c r="R55" s="3"/>
+      <c r="S55" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4585,13 +5376,16 @@
       <c r="V55" s="3"/>
       <c r="W55" s="3"/>
       <c r="X55" s="3"/>
-      <c r="Y55" s="3"/>
+      <c r="Y55" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z55" s="2"/>
       <c r="AA55" s="3"/>
       <c r="AB55" s="3"/>
       <c r="AC55" s="3"/>
       <c r="AD55" s="3"/>
-      <c r="AE55" s="3"/>
+      <c r="AE55" s="5"/>
       <c r="AF55" s="2"/>
       <c r="AG55" s="3"/>
       <c r="AH55" s="3"/>
@@ -4605,15 +5399,14 @@
       <c r="AP55" s="3"/>
       <c r="AQ55" s="3"/>
       <c r="AR55" s="2"/>
-      <c r="AS55" s="3"/>
-      <c r="AT55" s="3"/>
-      <c r="AU55" s="3"/>
-      <c r="AV55" s="3"/>
-      <c r="AW55" s="5"/>
+      <c r="AW55">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="56" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B56" s="2"/>
       <c r="C56" s="3"/>
@@ -4633,7 +5426,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S56">
+      <c r="N56" s="2"/>
+      <c r="O56" s="3"/>
+      <c r="P56" s="3"/>
+      <c r="Q56" s="3"/>
+      <c r="R56" s="3"/>
+      <c r="S56" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4642,13 +5440,16 @@
       <c r="V56" s="3"/>
       <c r="W56" s="3"/>
       <c r="X56" s="3"/>
-      <c r="Y56" s="3"/>
+      <c r="Y56" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z56" s="2"/>
       <c r="AA56" s="3"/>
       <c r="AB56" s="3"/>
       <c r="AC56" s="3"/>
       <c r="AD56" s="3"/>
-      <c r="AE56" s="3"/>
+      <c r="AE56" s="5"/>
       <c r="AF56" s="2"/>
       <c r="AG56" s="3"/>
       <c r="AH56" s="3"/>
@@ -4662,15 +5463,14 @@
       <c r="AP56" s="3"/>
       <c r="AQ56" s="3"/>
       <c r="AR56" s="2"/>
-      <c r="AS56" s="3"/>
-      <c r="AT56" s="3"/>
-      <c r="AU56" s="3"/>
-      <c r="AV56" s="3"/>
-      <c r="AW56" s="5"/>
+      <c r="AW56">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="57" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="B57" s="2"/>
       <c r="C57" s="3"/>
@@ -4690,7 +5490,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S57">
+      <c r="N57" s="2"/>
+      <c r="O57" s="3"/>
+      <c r="P57" s="3"/>
+      <c r="Q57" s="3"/>
+      <c r="R57" s="3"/>
+      <c r="S57" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4699,13 +5504,16 @@
       <c r="V57" s="3"/>
       <c r="W57" s="3"/>
       <c r="X57" s="3"/>
-      <c r="Y57" s="3"/>
+      <c r="Y57" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z57" s="2"/>
       <c r="AA57" s="3"/>
       <c r="AB57" s="3"/>
       <c r="AC57" s="3"/>
       <c r="AD57" s="3"/>
-      <c r="AE57" s="3"/>
+      <c r="AE57" s="5"/>
       <c r="AF57" s="2"/>
       <c r="AG57" s="3"/>
       <c r="AH57" s="3"/>
@@ -4719,15 +5527,14 @@
       <c r="AP57" s="3"/>
       <c r="AQ57" s="3"/>
       <c r="AR57" s="2"/>
-      <c r="AS57" s="3"/>
-      <c r="AT57" s="3"/>
-      <c r="AU57" s="3"/>
-      <c r="AV57" s="3"/>
-      <c r="AW57" s="5"/>
+      <c r="AW57">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="58" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B58" s="2"/>
       <c r="C58" s="3"/>
@@ -4747,7 +5554,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S58">
+      <c r="N58" s="2"/>
+      <c r="O58" s="3"/>
+      <c r="P58" s="3"/>
+      <c r="Q58" s="3"/>
+      <c r="R58" s="3"/>
+      <c r="S58" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4756,13 +5568,16 @@
       <c r="V58" s="3"/>
       <c r="W58" s="3"/>
       <c r="X58" s="3"/>
-      <c r="Y58" s="3"/>
+      <c r="Y58" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z58" s="2"/>
       <c r="AA58" s="3"/>
       <c r="AB58" s="3"/>
       <c r="AC58" s="3"/>
       <c r="AD58" s="3"/>
-      <c r="AE58" s="3"/>
+      <c r="AE58" s="5"/>
       <c r="AF58" s="2"/>
       <c r="AG58" s="3"/>
       <c r="AH58" s="3"/>
@@ -4776,15 +5591,14 @@
       <c r="AP58" s="3"/>
       <c r="AQ58" s="3"/>
       <c r="AR58" s="2"/>
-      <c r="AS58" s="3"/>
-      <c r="AT58" s="3"/>
-      <c r="AU58" s="3"/>
-      <c r="AV58" s="3"/>
-      <c r="AW58" s="5"/>
+      <c r="AW58">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="59" spans="1:49" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="B59" s="2"/>
       <c r="C59" s="3"/>
@@ -4804,7 +5618,12 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S59">
+      <c r="N59" s="2"/>
+      <c r="O59" s="3"/>
+      <c r="P59" s="3"/>
+      <c r="Q59" s="3"/>
+      <c r="R59" s="3"/>
+      <c r="S59" s="3">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -4813,13 +5632,16 @@
       <c r="V59" s="3"/>
       <c r="W59" s="3"/>
       <c r="X59" s="3"/>
-      <c r="Y59" s="3"/>
+      <c r="Y59" s="3">
+        <f t="shared" si="3"/>
+        <v>0</v>
+      </c>
       <c r="Z59" s="2"/>
       <c r="AA59" s="3"/>
       <c r="AB59" s="3"/>
       <c r="AC59" s="3"/>
       <c r="AD59" s="3"/>
-      <c r="AE59" s="3"/>
+      <c r="AE59" s="5"/>
       <c r="AF59" s="2"/>
       <c r="AG59" s="3"/>
       <c r="AH59" s="3"/>
@@ -4833,32 +5655,32 @@
       <c r="AP59" s="3"/>
       <c r="AQ59" s="3"/>
       <c r="AR59" s="2"/>
-      <c r="AS59" s="3"/>
-      <c r="AT59" s="3"/>
-      <c r="AU59" s="3"/>
-      <c r="AV59" s="3"/>
-      <c r="AW59" s="5"/>
+      <c r="AW59">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
     </row>
     <row r="60" spans="1:49" x14ac:dyDescent="0.25">
       <c r="M60" s="5">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S60">
-        <f t="shared" si="2"/>
+      <c r="AR60" s="2"/>
+      <c r="AW60">
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="8">
-    <mergeCell ref="AF1:AK1"/>
-    <mergeCell ref="AL1:AQ1"/>
-    <mergeCell ref="AR1:AW1"/>
-    <mergeCell ref="B1:G1"/>
-    <mergeCell ref="H1:M1"/>
     <mergeCell ref="N1:S1"/>
     <mergeCell ref="T1:Y1"/>
     <mergeCell ref="Z1:AE1"/>
+    <mergeCell ref="B1:G1"/>
+    <mergeCell ref="H1:M1"/>
+    <mergeCell ref="AR1:AW1"/>
+    <mergeCell ref="AF1:AK1"/>
+    <mergeCell ref="AL1:AQ1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>

</xml_diff>